<commit_message>
Macro is added to insert result into another sheet
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BRTC\2-DATEWISE TESTS\27-30-01-2021\1-B110227239-CE-20-21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6741A0D7-B4B2-47EF-9656-3D0A437C41EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FBF79-A976-4D06-A06E-33C0CB717F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="3610" windowWidth="14400" windowHeight="7270" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="50" r:id="rId1"/>
     <sheet name="Report" sheetId="51" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">main!$A$1:$L$132</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">main!$A$1:$M$132</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Report!$A$1:$I$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -25,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1144,6 +1145,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1162,6 +1172,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1182,18 +1195,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1395,7 +1396,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
@@ -1419,19 +1420,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.714413208389111</c:v>
+                  <c:v>43.268866135760327</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.782909930715938</c:v>
+                  <c:v>41.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.975914362176667</c:v>
+                  <c:v>40.76655052264806</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.65961945031713</c:v>
+                  <c:v>39.55584164789186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.844040762073561</c:v>
+                  <c:v>38.274831964152348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,6 +2033,121 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="main"/>
+      <sheetName val="input-output"/>
+      <sheetName val="Some Calculations"/>
+      <sheetName val="Report"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="24">
+          <cell r="D24">
+            <v>15</v>
+          </cell>
+          <cell r="E24">
+            <v>20</v>
+          </cell>
+          <cell r="F24">
+            <v>25</v>
+          </cell>
+          <cell r="G24">
+            <v>30</v>
+          </cell>
+          <cell r="H24">
+            <v>35</v>
+          </cell>
+          <cell r="M24">
+            <v>9.32</v>
+          </cell>
+          <cell r="N24">
+            <v>9.14</v>
+          </cell>
+          <cell r="O24">
+            <v>10.210000000000001</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="D25">
+            <v>10.88</v>
+          </cell>
+          <cell r="E25">
+            <v>7.75</v>
+          </cell>
+          <cell r="F25">
+            <v>9.0500000000000007</v>
+          </cell>
+          <cell r="G25">
+            <v>6.87</v>
+          </cell>
+          <cell r="H25">
+            <v>7.24</v>
+          </cell>
+          <cell r="M25">
+            <v>45.08</v>
+          </cell>
+          <cell r="N25">
+            <v>47.36</v>
+          </cell>
+          <cell r="O25">
+            <v>46.61</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="D26">
+            <v>48.66</v>
+          </cell>
+          <cell r="E26">
+            <v>47.51</v>
+          </cell>
+          <cell r="F26">
+            <v>45.41</v>
+          </cell>
+          <cell r="G26">
+            <v>50.23</v>
+          </cell>
+          <cell r="H26">
+            <v>44.27</v>
+          </cell>
+          <cell r="M26">
+            <v>38.880000000000003</v>
+          </cell>
+          <cell r="N26">
+            <v>40.770000000000003</v>
+          </cell>
+          <cell r="O26">
+            <v>40.32</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="D27">
+            <v>37.25</v>
+          </cell>
+          <cell r="E27">
+            <v>35.75</v>
+          </cell>
+          <cell r="F27">
+            <v>34.880000000000003</v>
+          </cell>
+          <cell r="G27">
+            <v>37.94</v>
+          </cell>
+          <cell r="H27">
+            <v>34.020000000000003</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2380,41 +2496,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A45" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" customWidth="1"/>
+    <col min="16" max="16" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="131" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="128"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="131" t="s">
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="130" t="s">
+      <c r="G8" s="133" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="130"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H8" s="133"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>29</v>
       </c>
@@ -2424,26 +2541,26 @@
       <c r="C9" s="75"/>
       <c r="D9" s="75"/>
       <c r="E9" s="75"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F9" s="134"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="130"/>
-      <c r="H10" s="130"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
         <v>30</v>
       </c>
@@ -2453,15 +2570,15 @@
       <c r="C11" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="D11" s="135" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="132"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="130"/>
-      <c r="H11" s="130"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E11" s="135"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="133"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>32</v>
       </c>
@@ -2479,7 +2596,7 @@
       </c>
       <c r="H12" s="39"/>
     </row>
-    <row r="13" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
         <v>28</v>
       </c>
@@ -2498,7 +2615,7 @@
       <c r="H13" s="21"/>
       <c r="J13" s="20"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
@@ -2514,7 +2631,7 @@
       <c r="K14" s="56"/>
       <c r="L14" s="57"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
@@ -2542,24 +2659,29 @@
       <c r="K15" s="89"/>
       <c r="L15" s="91"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="32">
-        <v>16</v>
+        <f>'[1]input-output'!$D$24</f>
+        <v>15</v>
       </c>
       <c r="D16" s="33">
+        <f>'[1]input-output'!$E$24</f>
         <v>20</v>
       </c>
       <c r="E16" s="33">
+        <f>'[1]input-output'!$F$24</f>
         <v>25</v>
       </c>
       <c r="F16" s="33">
+        <f>'[1]input-output'!$G$24</f>
         <v>30</v>
       </c>
       <c r="G16" s="33">
+        <f>'[1]input-output'!$H$24</f>
         <v>35</v>
       </c>
       <c r="H16" s="1"/>
@@ -2570,25 +2692,30 @@
       <c r="K16" s="51"/>
       <c r="L16" s="93"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="34">
-        <v>11.49</v>
+        <f>'[1]input-output'!$D$25</f>
+        <v>10.88</v>
       </c>
       <c r="D17" s="34">
-        <v>10.42</v>
+        <f>'[1]input-output'!$E$25</f>
+        <v>7.75</v>
       </c>
       <c r="E17" s="34">
-        <v>9.6300000000000008</v>
+        <f>'[1]input-output'!$F$25</f>
+        <v>9.0500000000000007</v>
       </c>
       <c r="F17" s="34">
-        <v>7.82</v>
+        <f>'[1]input-output'!$G$25</f>
+        <v>6.87</v>
       </c>
       <c r="G17" s="34">
-        <v>7.04</v>
+        <f>'[1]input-output'!$H$25</f>
+        <v>7.24</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2598,25 +2725,30 @@
       <c r="K17" s="51"/>
       <c r="L17" s="93"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="34">
-        <v>42.8</v>
+        <f>'[1]input-output'!$D$26</f>
+        <v>48.66</v>
       </c>
       <c r="D18" s="34">
-        <v>40.25</v>
+        <f>'[1]input-output'!$E$26</f>
+        <v>47.51</v>
       </c>
       <c r="E18" s="34">
-        <v>40.340000000000003</v>
+        <f>'[1]input-output'!$F$26</f>
+        <v>45.41</v>
       </c>
       <c r="F18" s="34">
-        <v>40.14</v>
+        <f>'[1]input-output'!$G$26</f>
+        <v>50.23</v>
       </c>
       <c r="G18" s="34">
-        <v>37.700000000000003</v>
+        <f>'[1]input-output'!$H$26</f>
+        <v>44.27</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2626,25 +2758,30 @@
       <c r="K18" s="51"/>
       <c r="L18" s="93"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="34">
-        <v>33.9</v>
+        <f>'[1]input-output'!$D$27</f>
+        <v>37.25</v>
       </c>
       <c r="D19" s="34">
-        <v>32.07</v>
+        <f>'[1]input-output'!$E$27</f>
+        <v>35.75</v>
       </c>
       <c r="E19" s="34">
-        <v>32.049999999999997</v>
+        <f>'[1]input-output'!$F$27</f>
+        <v>34.880000000000003</v>
       </c>
       <c r="F19" s="34">
-        <v>31.47</v>
+        <f>'[1]input-output'!$G$27</f>
+        <v>37.94</v>
       </c>
       <c r="G19" s="34">
-        <v>29.61</v>
+        <f>'[1]input-output'!$H$27</f>
+        <v>34.020000000000003</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2654,30 +2791,30 @@
       <c r="K19" s="51"/>
       <c r="L19" s="93"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>8.8999999999999986</v>
+        <v>11.409999999999997</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>8.18</v>
+        <v>11.759999999999998</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>8.2900000000000063</v>
+        <v>10.529999999999994</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>8.6700000000000017</v>
+        <v>12.29</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>8.0900000000000034</v>
+        <v>10.25</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2687,30 +2824,30 @@
       <c r="K20" s="51"/>
       <c r="L20" s="93"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>22.409999999999997</v>
+        <v>26.369999999999997</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>21.65</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>22.419999999999995</v>
+        <v>25.830000000000002</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>23.65</v>
+        <v>31.069999999999997</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>22.57</v>
+        <v>26.78</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2723,30 +2860,30 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>39.714413208389111</v>
+        <v>43.268866135760327</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>37.782909930715938</v>
+        <v>41.999999999999993</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>36.975914362176667</v>
+        <v>40.76655052264806</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>36.65961945031713</v>
+        <v>39.55584164789186</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>35.844040762073561</v>
+        <v>38.274831964152348</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -2759,7 +2896,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2778,7 +2915,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2797,7 +2934,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I25" s="95" t="s">
         <v>59</v>
       </c>
@@ -2808,7 +2945,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I26" s="95" t="s">
         <v>45</v>
       </c>
@@ -2819,7 +2956,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G27" s="15"/>
       <c r="I27" s="95" t="s">
         <v>46</v>
@@ -2831,7 +2968,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G28" s="13"/>
       <c r="H28" s="14"/>
       <c r="I28" s="99" t="s">
@@ -2844,7 +2981,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I29" s="97" t="s">
         <v>61</v>
       </c>
@@ -2855,61 +2992,61 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
       <c r="K30" s="35"/>
       <c r="L30" s="35"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
       <c r="K31" s="35"/>
       <c r="L31" s="35"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
       <c r="K32" s="35"/>
       <c r="L32" s="35"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
       <c r="K33" s="35"/>
       <c r="L33" s="35"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I34" s="35"/>
       <c r="J34" s="53"/>
       <c r="K34" s="53"/>
       <c r="L34" s="35"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I35" s="35"/>
       <c r="J35" s="35"/>
       <c r="K35" s="35"/>
       <c r="L35" s="53"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="I36" s="35"/>
       <c r="J36" s="28"/>
       <c r="K36" s="35"/>
       <c r="L36" s="35"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I37" s="35"/>
       <c r="J37" s="35"/>
       <c r="K37" s="35"/>
       <c r="L37" s="35"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I38" s="35"/>
       <c r="J38" s="35"/>
       <c r="K38" s="35"/>
       <c r="L38" s="35"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="D39" s="62" t="s">
         <v>49</v>
       </c>
@@ -2917,14 +3054,14 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>1.2415076130079297</v>
+        <v>1.4900057940109022</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
       <c r="K39" s="35"/>
       <c r="L39" s="35"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="D40" s="62" t="s">
         <v>27</v>
       </c>
@@ -2932,7 +3069,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -2942,7 +3079,7 @@
       <c r="K40" s="35"/>
       <c r="L40" s="35"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="D41" s="62" t="s">
         <v>48</v>
       </c>
@@ -2950,16 +3087,16 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>10.471139978355467</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>13.422766596204029</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="17"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -2976,58 +3113,67 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="9"/>
       <c r="D44" s="36">
-        <v>9.4600000000000009</v>
+        <f>'[1]input-output'!$M$24</f>
+        <v>9.32</v>
       </c>
       <c r="E44" s="36">
-        <v>10.31</v>
+        <f>'[1]input-output'!$N$24</f>
+        <v>9.14</v>
       </c>
       <c r="F44" s="34">
-        <v>7.45</v>
+        <f>'[1]input-output'!$O$24</f>
+        <v>10.210000000000001</v>
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B45" s="25"/>
       <c r="C45" s="7"/>
       <c r="D45" s="36">
-        <v>39.74</v>
+        <f>'[1]input-output'!$M$25</f>
+        <v>45.08</v>
       </c>
       <c r="E45" s="36">
-        <v>40.35</v>
+        <f>'[1]input-output'!$N$25</f>
+        <v>47.36</v>
       </c>
       <c r="F45" s="34">
-        <v>38.85</v>
+        <f>'[1]input-output'!$O$25</f>
+        <v>46.61</v>
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="27"/>
       <c r="D46" s="36">
-        <v>33.9</v>
+        <f>'[1]input-output'!$M$26</f>
+        <v>38.880000000000003</v>
       </c>
       <c r="E46" s="36">
-        <v>34.58</v>
+        <f>'[1]input-output'!$N$26</f>
+        <v>40.770000000000003</v>
       </c>
       <c r="F46" s="34">
-        <v>32.78</v>
+        <f>'[1]input-output'!$O$26</f>
+        <v>40.32</v>
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>11</v>
       </c>
@@ -3035,19 +3181,19 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>5.8400000000000034</v>
+        <v>6.1999999999999957</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>5.7700000000000031</v>
+        <v>6.5899999999999963</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>6.07</v>
+        <v>6.2899999999999991</v>
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>12</v>
       </c>
@@ -3055,19 +3201,19 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>24.439999999999998</v>
+        <v>29.560000000000002</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>24.269999999999996</v>
+        <v>31.630000000000003</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>25.330000000000002</v>
+        <v>30.11</v>
       </c>
       <c r="G48" s="16"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -3075,18 +3221,18 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>23.895253682487741</v>
+        <v>20.974289580514192</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>23.774206839719835</v>
+        <v>20.83465064811886</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>23.963679431504143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>20.890069744271003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="41"/>
@@ -3094,7 +3240,7 @@
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="41"/>
       <c r="B51" s="41"/>
       <c r="C51" s="41"/>
@@ -3102,7 +3248,7 @@
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
       <c r="C52" s="41"/>
@@ -3110,7 +3256,7 @@
       <c r="E52" s="48"/>
       <c r="F52" s="48"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="41"/>
@@ -3118,26 +3264,26 @@
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="E54" s="66" t="s">
         <v>16</v>
       </c>
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E55" s="63"/>
       <c r="F55" s="63"/>
       <c r="G55" s="63"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A56" s="29"/>
       <c r="E56" s="66" t="s">
         <v>26</v>
@@ -3145,13 +3291,13 @@
       <c r="F56" s="63"/>
       <c r="G56" s="67">
         <f>G40-G54</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>20</v>
       </c>
@@ -3162,9 +3308,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="73" t="s">
         <v>71</v>
       </c>
@@ -3178,7 +3324,7 @@
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="74" t="s">
         <v>23</v>
       </c>
@@ -3192,7 +3338,7 @@
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="74" t="s">
         <v>22</v>
       </c>
@@ -3206,7 +3352,7 @@
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="74" t="s">
         <v>24</v>
       </c>
@@ -3220,31 +3366,31 @@
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
     </row>
-    <row r="126" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H127" s="1"/>
     </row>
-    <row r="129" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H129" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H130" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H131" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H133" s="1"/>
     </row>
   </sheetData>
@@ -3259,11 +3405,11 @@
   <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="64" max="11" man="1"/>
+    <brk id="64" max="12" man="1"/>
     <brk id="118" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="8" max="134" man="1"/>
+    <brk id="8" max="131" man="1"/>
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3271,88 +3417,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A7:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="10" max="10" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="133"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="138" t="str">
+      <c r="B8" s="142" t="str">
         <f>main!B8</f>
         <v>1102-27239/CE/20-21 Dated 20/01/2021</v>
       </c>
-      <c r="C8" s="138"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="139" t="s">
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="142" t="str">
+      <c r="G8" s="137" t="str">
         <f>main!G8</f>
         <v>Cladding Soil Tests of Padma Bridge Rail Link Project; Sampling Source: Along the Alignment &amp; Stockpile (Sections 02, 03 &amp; 04)</v>
       </c>
-      <c r="H8" s="142"/>
-      <c r="I8" s="142"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" s="137"/>
+      <c r="I8" s="137"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="141" t="str">
+      <c r="B9" s="128" t="str">
         <f>main!B9</f>
         <v>Md. Shahin Kadir, On behalf of Project Manager-3, CSC, Phase-2, PBRLP</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
-      <c r="F9" s="139"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" s="143"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="140" t="str">
+      <c r="B10" s="144" t="str">
         <f>main!B10</f>
         <v>609/Project/21/PBRLP Dated 20/01/2021</v>
       </c>
-      <c r="C10" s="140"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="139"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="142"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="144"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="137"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
         <v>30</v>
       </c>
@@ -3363,17 +3510,17 @@
       <c r="C11" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="141" t="str">
+      <c r="D11" s="128" t="str">
         <f>main!D11</f>
         <v>Bag No.13;Ch. 31+500;Section-2</v>
       </c>
       <c r="E11" s="126"/>
-      <c r="F11" s="139"/>
-      <c r="G11" s="142"/>
-      <c r="H11" s="142"/>
-      <c r="I11" s="142"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11" s="143"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="137"/>
+      <c r="I11" s="137"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>32</v>
       </c>
@@ -3388,12 +3535,12 @@
       <c r="G12" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="143" t="str">
+      <c r="H12" s="129" t="str">
         <f>main!G12</f>
         <v>26/01/2021</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>28</v>
       </c>
@@ -3408,12 +3555,12 @@
       <c r="G13" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="144" t="str">
+      <c r="H13" s="130" t="str">
         <f>main!G13</f>
         <v>ASTM D4318, D4943</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
@@ -3423,7 +3570,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="76"/>
       <c r="B15" s="76"/>
       <c r="C15" s="77"/>
@@ -3434,14 +3581,14 @@
       <c r="H15" s="79"/>
       <c r="I15" s="80"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="69"/>
       <c r="C16" s="70">
         <f>main!C16</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="70">
         <f>main!D16</f>
@@ -3462,175 +3609,175 @@
       <c r="H16" s="69"/>
       <c r="I16" s="83"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>11.49</v>
+        <v>10.88</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>10.42</v>
+        <v>7.75</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>9.6300000000000008</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>7.82</v>
+        <v>6.87</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>7.04</v>
+        <v>7.24</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>42.8</v>
+        <v>48.66</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>40.25</v>
+        <v>47.51</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>40.340000000000003</v>
+        <v>45.41</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>40.14</v>
+        <v>50.23</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>37.700000000000003</v>
+        <v>44.27</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>33.9</v>
+        <v>37.25</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>32.07</v>
+        <v>35.75</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>32.049999999999997</v>
+        <v>34.880000000000003</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>31.47</v>
+        <v>37.94</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>29.61</v>
+        <v>34.020000000000003</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A20" s="69" t="s">
         <v>51</v>
       </c>
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>8.8999999999999986</v>
+        <v>11.409999999999997</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>8.18</v>
+        <v>11.759999999999998</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>8.2900000000000063</v>
+        <v>10.529999999999994</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>8.6700000000000017</v>
+        <v>12.29</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>8.0900000000000034</v>
+        <v>10.25</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A21" s="69" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>22.409999999999997</v>
+        <v>26.369999999999997</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>21.65</v>
+        <v>28</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>22.419999999999995</v>
+        <v>25.830000000000002</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>23.65</v>
+        <v>31.069999999999997</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>22.57</v>
+        <v>26.78</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>39.714413208389111</v>
+        <v>43.268866135760327</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>37.782909930715938</v>
+        <v>41.999999999999993</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>36.975914362176667</v>
+        <v>40.76655052264806</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>36.65961945031713</v>
+        <v>39.55584164789186</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>35.844040762073561</v>
+        <v>38.274831964152348</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="84"/>
       <c r="B23" s="84"/>
       <c r="C23" s="84"/>
@@ -3641,7 +3788,7 @@
       <c r="H23" s="84"/>
       <c r="I23" s="83"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="84"/>
       <c r="B24" s="84"/>
       <c r="C24" s="84"/>
@@ -3652,7 +3799,7 @@
       <c r="H24" s="84"/>
       <c r="I24" s="83"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="83"/>
       <c r="B25" s="83"/>
       <c r="C25" s="83"/>
@@ -3663,7 +3810,7 @@
       <c r="H25" s="83"/>
       <c r="I25" s="83"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="83"/>
       <c r="B26" s="83"/>
       <c r="C26" s="83"/>
@@ -3674,7 +3821,7 @@
       <c r="H26" s="83"/>
       <c r="I26" s="83"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="83"/>
       <c r="B27" s="83"/>
       <c r="C27" s="83"/>
@@ -3685,7 +3832,7 @@
       <c r="H27" s="83"/>
       <c r="I27" s="83"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="80"/>
       <c r="B28" s="80"/>
       <c r="C28" s="80"/>
@@ -3696,7 +3843,7 @@
       <c r="H28" s="82"/>
       <c r="I28" s="80"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="80"/>
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
@@ -3707,7 +3854,7 @@
       <c r="H29" s="80"/>
       <c r="I29" s="80"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="80"/>
       <c r="B30" s="80"/>
       <c r="C30" s="80"/>
@@ -3718,10 +3865,10 @@
       <c r="H30" s="80"/>
       <c r="I30" s="80"/>
     </row>
-    <row r="35" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="124" t="s">
         <v>55</v>
       </c>
@@ -3729,7 +3876,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3738,38 +3885,38 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>10.47</v>
+        <v>13.42</v>
       </c>
       <c r="I36" s="68"/>
     </row>
-    <row r="37" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
     </row>
-    <row r="38" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
       <c r="D40" s="17"/>
       <c r="G40" s="19"/>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="17"/>
       <c r="G41" s="58"/>
     </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="17"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -3789,7 +3936,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>5</v>
       </c>
@@ -3797,19 +3944,19 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>9.4600000000000009</v>
+        <v>9.32</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>10.31</v>
+        <v>9.14</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>7.45</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>9</v>
       </c>
@@ -3817,15 +3964,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>39.74</v>
+        <v>45.08</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>40.35</v>
+        <v>47.36</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>38.85</v>
+        <v>46.61</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3833,10 +3980,10 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
@@ -3844,15 +3991,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>33.9</v>
+        <v>38.880000000000003</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>34.58</v>
+        <v>40.770000000000003</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>32.78</v>
+        <v>40.32</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -3860,10 +4007,10 @@
       <c r="H46" s="1"/>
       <c r="I46" s="121">
         <f>main!G56</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>11</v>
       </c>
@@ -3871,15 +4018,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>5.8400000000000034</v>
+        <v>6.1999999999999957</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>5.7700000000000031</v>
+        <v>6.5899999999999963</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>6.07</v>
+        <v>6.2899999999999991</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -3887,10 +4034,10 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>1.24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>12</v>
       </c>
@@ -3898,19 +4045,19 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>24.439999999999998</v>
+        <v>29.560000000000002</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>24.269999999999996</v>
+        <v>31.630000000000003</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>25.330000000000002</v>
+        <v>30.11</v>
       </c>
       <c r="G48" s="16"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -3918,18 +4065,18 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>23.895253682487741</v>
+        <v>20.974289580514192</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>23.774206839719835</v>
+        <v>20.83465064811886</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>23.963679431504143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20.890069744271003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="41"/>
@@ -3937,7 +4084,7 @@
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A51" s="30" t="s">
         <v>58</v>
       </c>
@@ -3949,7 +4096,7 @@
       <c r="G51" s="71"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="41"/>
       <c r="C52" s="71"/>
@@ -3957,7 +4104,7 @@
       <c r="E52" s="48"/>
       <c r="F52" s="48"/>
     </row>
-    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="106" t="str">
         <f>main!I25</f>
         <v>Shrinkage Limit (%):</v>
@@ -3979,7 +4126,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="106" t="str">
         <f>main!I26</f>
         <v>Shrinkage Ratio:</v>
@@ -3991,14 +4138,14 @@
         <v>---</v>
       </c>
       <c r="E54" s="106"/>
-      <c r="F54" s="135" t="s">
+      <c r="F54" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="G54" s="136"/>
-      <c r="H54" s="136"/>
-      <c r="I54" s="137"/>
-    </row>
-    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G54" s="140"/>
+      <c r="H54" s="140"/>
+      <c r="I54" s="141"/>
+    </row>
+    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="106" t="str">
         <f>main!I27</f>
         <v>Volumetric Shrinkage (%):</v>
@@ -4020,7 +4167,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="106" t="str">
         <f>main!I28</f>
         <v>Linear Shrinkage (%):</v>
@@ -4042,15 +4189,15 @@
         <v>---</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="134" t="s">
+    <row r="57" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="134"/>
+      <c r="B57" s="138"/>
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.24299999999999999</v>
+        <v>0.27899999999999997</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>
@@ -4058,7 +4205,7 @@
       <c r="H57" s="24"/>
       <c r="I57" s="24"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>20</v>
       </c>
@@ -4070,9 +4217,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="str">
         <f>main!A61</f>
         <v>Dr. A. B. M. Badruzzaman</v>
@@ -4083,7 +4230,7 @@
         <v>Dr. Md. Ferdous Alam</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="23" t="str">
         <f>main!A62</f>
         <v>Professor</v>
@@ -4094,7 +4241,7 @@
         <v>Assistant Professor</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="str">
         <f>main!A63</f>
         <v>Department of Civil Engineering</v>
@@ -4105,7 +4252,7 @@
         <v>Department of Civil Engineering</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="str">
         <f>main!A64</f>
         <v>BUET, Dhaka - 1000.</v>
@@ -4116,31 +4263,31 @@
         <v>BUET, Dhaka - 1000.</v>
       </c>
     </row>
-    <row r="126" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H127" s="1"/>
     </row>
-    <row r="129" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H129" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H130" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H131" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H133" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
22 data calculated upto broing no 87 and D-20
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8CA055-9235-4C1E-AF1E-84C11ED9F3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A03704-6F40-4749-A219-2C9DF3D8BF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9970" yWindow="180" windowWidth="8840" windowHeight="9090" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="50" r:id="rId1"/>
@@ -1399,16 +1399,16 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1420,19 +1420,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.393986121819601</c:v>
+                  <c:v>37.986361813076606</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.495367070563084</c:v>
+                  <c:v>38.427734375000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.846777462505067</c:v>
+                  <c:v>36.530214424951282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.274210713018817</c:v>
+                  <c:v>39.103182256509136</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.789922193404969</c:v>
+                  <c:v>35.6826241134752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,94 +2050,94 @@
             <v>15</v>
           </cell>
           <cell r="E24">
-            <v>20</v>
+            <v>19</v>
           </cell>
           <cell r="F24">
-            <v>26</v>
+            <v>24</v>
           </cell>
           <cell r="G24">
-            <v>30</v>
+            <v>29</v>
           </cell>
           <cell r="H24">
-            <v>35</v>
+            <v>34</v>
           </cell>
           <cell r="M24">
-            <v>9.9499999999999993</v>
+            <v>7.02</v>
           </cell>
           <cell r="N24">
-            <v>10.08</v>
+            <v>11.18</v>
           </cell>
           <cell r="O24">
-            <v>8.6999999999999993</v>
+            <v>9.09</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25">
-            <v>7.5</v>
+            <v>10.16</v>
           </cell>
           <cell r="E25">
-            <v>7.41</v>
+            <v>8.9600000000000009</v>
           </cell>
           <cell r="F25">
-            <v>10.94</v>
+            <v>9.83</v>
           </cell>
           <cell r="G25">
-            <v>9.61</v>
+            <v>9.6999999999999993</v>
           </cell>
           <cell r="H25">
-            <v>7.33</v>
+            <v>10.23</v>
           </cell>
           <cell r="M25">
-            <v>46.98</v>
+            <v>45.45</v>
           </cell>
           <cell r="N25">
-            <v>47.72</v>
+            <v>47.74</v>
           </cell>
           <cell r="O25">
-            <v>42.19</v>
+            <v>44.72</v>
           </cell>
         </row>
         <row r="26">
           <cell r="D26">
-            <v>43.14</v>
+            <v>44.56</v>
           </cell>
           <cell r="E26">
-            <v>45.43</v>
+            <v>37.31</v>
           </cell>
           <cell r="F26">
-            <v>43.96</v>
+            <v>44.85</v>
           </cell>
           <cell r="G26">
-            <v>47.18</v>
+            <v>38.549999999999997</v>
           </cell>
           <cell r="H26">
-            <v>43.17</v>
+            <v>40.840000000000003</v>
           </cell>
           <cell r="M26">
-            <v>40.450000000000003</v>
+            <v>38</v>
           </cell>
           <cell r="N26">
-            <v>41.02</v>
+            <v>40.659999999999997</v>
           </cell>
           <cell r="O26">
-            <v>36.32</v>
+            <v>37.86</v>
           </cell>
         </row>
         <row r="27">
           <cell r="D27">
-            <v>33.44</v>
+            <v>35.090000000000003</v>
           </cell>
           <cell r="E27">
-            <v>35.47</v>
+            <v>29.44</v>
           </cell>
           <cell r="F27">
-            <v>35.61</v>
+            <v>35.479999999999997</v>
           </cell>
           <cell r="G27">
-            <v>37.799999999999997</v>
+            <v>30.44</v>
           </cell>
           <cell r="H27">
-            <v>34.32</v>
+            <v>32.79</v>
           </cell>
         </row>
       </sheetData>
@@ -2501,7 +2501,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -2672,19 +2672,19 @@
       </c>
       <c r="D16" s="33">
         <f>'[1]input-output'!$E$24</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="33">
         <f>'[1]input-output'!$F$24</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F16" s="33">
         <f>'[1]input-output'!$G$24</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="33">
         <f>'[1]input-output'!$H$24</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="92" t="s">
@@ -2701,23 +2701,23 @@
       <c r="B17" s="4"/>
       <c r="C17" s="34">
         <f>'[1]input-output'!$D$25</f>
-        <v>7.5</v>
+        <v>10.16</v>
       </c>
       <c r="D17" s="34">
         <f>'[1]input-output'!$E$25</f>
-        <v>7.41</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="E17" s="34">
         <f>'[1]input-output'!$F$25</f>
-        <v>10.94</v>
+        <v>9.83</v>
       </c>
       <c r="F17" s="34">
         <f>'[1]input-output'!$G$25</f>
-        <v>9.61</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="G17" s="34">
         <f>'[1]input-output'!$H$25</f>
-        <v>7.33</v>
+        <v>10.23</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2734,23 +2734,23 @@
       <c r="B18" s="12"/>
       <c r="C18" s="34">
         <f>'[1]input-output'!$D$26</f>
-        <v>43.14</v>
+        <v>44.56</v>
       </c>
       <c r="D18" s="34">
         <f>'[1]input-output'!$E$26</f>
-        <v>45.43</v>
+        <v>37.31</v>
       </c>
       <c r="E18" s="34">
         <f>'[1]input-output'!$F$26</f>
-        <v>43.96</v>
+        <v>44.85</v>
       </c>
       <c r="F18" s="34">
         <f>'[1]input-output'!$G$26</f>
-        <v>47.18</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="G18" s="34">
         <f>'[1]input-output'!$H$26</f>
-        <v>43.17</v>
+        <v>40.840000000000003</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2767,23 +2767,23 @@
       <c r="B19" s="4"/>
       <c r="C19" s="34">
         <f>'[1]input-output'!$D$27</f>
-        <v>33.44</v>
+        <v>35.090000000000003</v>
       </c>
       <c r="D19" s="34">
         <f>'[1]input-output'!$E$27</f>
-        <v>35.47</v>
+        <v>29.44</v>
       </c>
       <c r="E19" s="34">
         <f>'[1]input-output'!$F$27</f>
-        <v>35.61</v>
+        <v>35.479999999999997</v>
       </c>
       <c r="F19" s="34">
         <f>'[1]input-output'!$G$27</f>
-        <v>37.799999999999997</v>
+        <v>30.44</v>
       </c>
       <c r="G19" s="34">
         <f>'[1]input-output'!$H$27</f>
-        <v>34.32</v>
+        <v>32.79</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2800,23 +2800,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>9.7000000000000028</v>
+        <v>9.4699999999999989</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>9.9600000000000009</v>
+        <v>7.870000000000001</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>8.3500000000000014</v>
+        <v>9.3700000000000045</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>9.3800000000000026</v>
+        <v>8.1099999999999959</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>8.8500000000000014</v>
+        <v>8.0500000000000043</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2833,23 +2833,23 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>25.939999999999998</v>
+        <v>24.930000000000003</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>28.06</v>
+        <v>20.48</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>24.67</v>
+        <v>25.65</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>28.189999999999998</v>
+        <v>20.740000000000002</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>26.990000000000002</v>
+        <v>22.56</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2869,23 +2869,23 @@
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>37.393986121819601</v>
+        <v>37.986361813076606</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>35.495367070563084</v>
+        <v>38.427734375000007</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>33.846777462505067</v>
+        <v>36.530214424951282</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>33.274210713018817</v>
+        <v>39.103182256509136</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>32.789922193404969</v>
+        <v>35.6826241134752</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -3056,7 +3056,7 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>1.016138625202397</v>
+        <v>3.142590140844304</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -3071,7 +3071,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -3089,7 +3089,7 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>12.793530014087034</v>
+        <v>4.1367150717615866</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.3">
@@ -3123,15 +3123,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="36">
         <f>'[1]input-output'!$M$24</f>
-        <v>9.9499999999999993</v>
+        <v>7.02</v>
       </c>
       <c r="E44" s="36">
         <f>'[1]input-output'!$N$24</f>
-        <v>10.08</v>
+        <v>11.18</v>
       </c>
       <c r="F44" s="34">
         <f>'[1]input-output'!$O$24</f>
-        <v>8.6999999999999993</v>
+        <v>9.09</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3143,15 +3143,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="36">
         <f>'[1]input-output'!$M$25</f>
-        <v>46.98</v>
+        <v>45.45</v>
       </c>
       <c r="E45" s="36">
         <f>'[1]input-output'!$N$25</f>
-        <v>47.72</v>
+        <v>47.74</v>
       </c>
       <c r="F45" s="34">
         <f>'[1]input-output'!$O$25</f>
-        <v>42.19</v>
+        <v>44.72</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3163,15 +3163,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="36">
         <f>'[1]input-output'!$M$26</f>
-        <v>40.450000000000003</v>
+        <v>38</v>
       </c>
       <c r="E46" s="36">
         <f>'[1]input-output'!$N$26</f>
-        <v>41.02</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="F46" s="34">
         <f>'[1]input-output'!$O$26</f>
-        <v>36.32</v>
+        <v>37.86</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3183,15 +3183,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>6.529999999999994</v>
+        <v>7.4500000000000028</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>6.6999999999999957</v>
+        <v>7.0800000000000054</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>5.8699999999999974</v>
+        <v>6.8599999999999994</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3203,15 +3203,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>30.500000000000004</v>
+        <v>30.98</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>30.940000000000005</v>
+        <v>29.479999999999997</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>27.62</v>
+        <v>28.77</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -3223,15 +3223,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>21.409836065573749</v>
+        <v>24.047772756617181</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>21.654815772462815</v>
+        <v>24.016282225237472</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>21.252715423606073</v>
+        <v>23.844282238442823</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
@@ -3422,8 +3422,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A7:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C31" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C16" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3594,19 +3594,19 @@
       </c>
       <c r="D16" s="70">
         <f>main!D16</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="70">
         <f>main!E16</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F16" s="70">
         <f>main!F16</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="70">
         <f>main!G16</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="69"/>
       <c r="I16" s="83"/>
@@ -3618,23 +3618,23 @@
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>7.5</v>
+        <v>10.16</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>7.41</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>10.94</v>
+        <v>9.83</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>9.61</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>7.33</v>
+        <v>10.23</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
@@ -3646,23 +3646,23 @@
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>43.14</v>
+        <v>44.56</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>45.43</v>
+        <v>37.31</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>43.96</v>
+        <v>44.85</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>47.18</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>43.17</v>
+        <v>40.840000000000003</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
@@ -3674,23 +3674,23 @@
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>33.44</v>
+        <v>35.090000000000003</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>35.47</v>
+        <v>29.44</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>35.61</v>
+        <v>35.479999999999997</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>37.799999999999997</v>
+        <v>30.44</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>34.32</v>
+        <v>32.79</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
@@ -3702,23 +3702,23 @@
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>9.7000000000000028</v>
+        <v>9.4699999999999989</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>9.9600000000000009</v>
+        <v>7.870000000000001</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>8.3500000000000014</v>
+        <v>9.3700000000000045</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>9.3800000000000026</v>
+        <v>8.1099999999999959</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>8.8500000000000014</v>
+        <v>8.0500000000000043</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
@@ -3730,23 +3730,23 @@
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>25.939999999999998</v>
+        <v>24.930000000000003</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>28.06</v>
+        <v>20.48</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>24.67</v>
+        <v>25.65</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>28.189999999999998</v>
+        <v>20.740000000000002</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>26.990000000000002</v>
+        <v>22.56</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
@@ -3758,23 +3758,23 @@
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>37.393986121819601</v>
+        <v>37.986361813076606</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>35.495367070563084</v>
+        <v>38.427734375000007</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>33.846777462505067</v>
+        <v>36.530214424951282</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>33.274210713018817</v>
+        <v>39.103182256509136</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>32.789922193404969</v>
+        <v>35.6826241134752</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
@@ -3878,7 +3878,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3887,7 +3887,7 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>12.79</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I36" s="68"/>
     </row>
@@ -3946,15 +3946,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>9.9499999999999993</v>
+        <v>7.02</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>10.08</v>
+        <v>11.18</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>8.6999999999999993</v>
+        <v>9.09</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3966,15 +3966,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>46.98</v>
+        <v>45.45</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>47.72</v>
+        <v>47.74</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>42.19</v>
+        <v>44.72</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3982,7 +3982,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -3993,15 +3993,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>40.450000000000003</v>
+        <v>38</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>41.02</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>36.32</v>
+        <v>37.86</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -4020,15 +4020,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>6.529999999999994</v>
+        <v>7.4500000000000028</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>6.6999999999999957</v>
+        <v>7.0800000000000054</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>5.8699999999999974</v>
+        <v>6.8599999999999994</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -4036,7 +4036,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>1.02</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4047,15 +4047,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>30.500000000000004</v>
+        <v>30.98</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>30.940000000000005</v>
+        <v>29.479999999999997</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>27.62</v>
+        <v>28.77</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -4067,15 +4067,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>21.409836065573749</v>
+        <v>24.047772756617181</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>21.654815772462815</v>
+        <v>24.016282225237472</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>21.252715423606073</v>
+        <v>23.844282238442823</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4199,7 +4199,7 @@
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.21599999999999997</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>

</xml_diff>

<commit_message>
Repo downloded to minaz's pc
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0753d6b33ebe78a/Desktop/thesis-repo/ann-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A03704-6F40-4749-A219-2C9DF3D8BF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="50" r:id="rId1"/>
@@ -28,7 +28,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2141,10 +2144,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2501,21 +2504,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" customWidth="1"/>
-    <col min="16" max="16" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>14</v>
       </c>
@@ -2533,7 +2536,7 @@
       </c>
       <c r="H8" s="133"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="44" t="s">
         <v>29</v>
       </c>
@@ -2547,7 +2550,7 @@
       <c r="G9" s="133"/>
       <c r="H9" s="133"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
         <v>25</v>
       </c>
@@ -2562,7 +2565,7 @@
       <c r="H10" s="133"/>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
         <v>30</v>
       </c>
@@ -2580,7 +2583,7 @@
       <c r="G11" s="133"/>
       <c r="H11" s="133"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>32</v>
       </c>
@@ -2598,7 +2601,7 @@
       </c>
       <c r="H12" s="39"/>
     </row>
-    <row r="13" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>28</v>
       </c>
@@ -2617,7 +2620,7 @@
       <c r="H13" s="21"/>
       <c r="J13" s="20"/>
     </row>
-    <row r="14" spans="1:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
@@ -2633,7 +2636,7 @@
       <c r="K14" s="56"/>
       <c r="L14" s="57"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
@@ -2661,7 +2664,7 @@
       <c r="K15" s="89"/>
       <c r="L15" s="91"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
@@ -2694,7 +2697,7 @@
       <c r="K16" s="51"/>
       <c r="L16" s="93"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -2727,7 +2730,7 @@
       <c r="K17" s="51"/>
       <c r="L17" s="93"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -2760,7 +2763,7 @@
       <c r="K18" s="51"/>
       <c r="L18" s="93"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -2793,7 +2796,7 @@
       <c r="K19" s="51"/>
       <c r="L19" s="93"/>
     </row>
-    <row r="20" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2829,7 @@
       <c r="K20" s="51"/>
       <c r="L20" s="93"/>
     </row>
-    <row r="21" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2917,7 +2920,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2936,7 +2939,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I25" s="95" t="s">
         <v>59</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I26" s="95" t="s">
         <v>45</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G27" s="15"/>
       <c r="I27" s="95" t="s">
         <v>46</v>
@@ -2970,7 +2973,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G28" s="13"/>
       <c r="H28" s="14"/>
       <c r="I28" s="99" t="s">
@@ -2983,7 +2986,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I29" s="97" t="s">
         <v>61</v>
       </c>
@@ -2994,61 +2997,61 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
       <c r="K30" s="35"/>
       <c r="L30" s="35"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
       <c r="K31" s="35"/>
       <c r="L31" s="35"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
       <c r="K32" s="35"/>
       <c r="L32" s="35"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
       <c r="K33" s="35"/>
       <c r="L33" s="35"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I34" s="35"/>
       <c r="J34" s="53"/>
       <c r="K34" s="53"/>
       <c r="L34" s="35"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I35" s="35"/>
       <c r="J35" s="35"/>
       <c r="K35" s="35"/>
       <c r="L35" s="53"/>
     </row>
-    <row r="36" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I36" s="35"/>
       <c r="J36" s="28"/>
       <c r="K36" s="35"/>
       <c r="L36" s="35"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I37" s="35"/>
       <c r="J37" s="35"/>
       <c r="K37" s="35"/>
       <c r="L37" s="35"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I38" s="35"/>
       <c r="J38" s="35"/>
       <c r="K38" s="35"/>
       <c r="L38" s="35"/>
     </row>
-    <row r="39" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D39" s="62" t="s">
         <v>49</v>
       </c>
@@ -3063,7 +3066,7 @@
       <c r="K39" s="35"/>
       <c r="L39" s="35"/>
     </row>
-    <row r="40" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D40" s="62" t="s">
         <v>27</v>
       </c>
@@ -3081,7 +3084,7 @@
       <c r="K40" s="35"/>
       <c r="L40" s="35"/>
     </row>
-    <row r="41" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D41" s="62" t="s">
         <v>48</v>
       </c>
@@ -3092,13 +3095,13 @@
         <v>4.1367150717615866</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="17"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -3115,7 +3118,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>5</v>
       </c>
@@ -3135,7 +3138,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>9</v>
       </c>
@@ -3155,7 +3158,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
@@ -3175,7 +3178,7 @@
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>11</v>
       </c>
@@ -3195,7 +3198,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>12</v>
       </c>
@@ -3215,7 +3218,7 @@
       </c>
       <c r="G48" s="16"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>23.844282238442823</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="41"/>
@@ -3242,7 +3245,7 @@
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="41"/>
       <c r="B51" s="41"/>
       <c r="C51" s="41"/>
@@ -3250,7 +3253,7 @@
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
       <c r="C52" s="41"/>
@@ -3258,7 +3261,7 @@
       <c r="E52" s="48"/>
       <c r="F52" s="48"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="41"/>
@@ -3266,7 +3269,7 @@
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
     </row>
-    <row r="54" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E54" s="66" t="s">
         <v>16</v>
       </c>
@@ -3279,13 +3282,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E55" s="63"/>
       <c r="F55" s="63"/>
       <c r="G55" s="63"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="29"/>
       <c r="E56" s="66" t="s">
         <v>26</v>
@@ -3299,7 +3302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>20</v>
       </c>
@@ -3310,9 +3313,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="73" t="s">
         <v>71</v>
       </c>
@@ -3326,7 +3329,7 @@
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="74" t="s">
         <v>23</v>
       </c>
@@ -3340,7 +3343,7 @@
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="74" t="s">
         <v>22</v>
       </c>
@@ -3354,7 +3357,7 @@
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="74" t="s">
         <v>24</v>
       </c>
@@ -3368,31 +3371,31 @@
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
     </row>
-    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H127" s="1"/>
     </row>
-    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H129" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H130" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H131" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H133" s="1"/>
     </row>
   </sheetData>
@@ -3422,20 +3425,20 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A7:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C16" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="C31" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="136" t="s">
         <v>50</v>
       </c>
@@ -3448,7 +3451,7 @@
       <c r="H7" s="136"/>
       <c r="I7" s="136"/>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
         <v>14</v>
       </c>
@@ -3469,7 +3472,7 @@
       <c r="H8" s="137"/>
       <c r="I8" s="137"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
         <v>29</v>
       </c>
@@ -3485,7 +3488,7 @@
       <c r="H9" s="137"/>
       <c r="I9" s="137"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
         <v>25</v>
       </c>
@@ -3501,7 +3504,7 @@
       <c r="H10" s="137"/>
       <c r="I10" s="137"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
         <v>30</v>
       </c>
@@ -3522,7 +3525,7 @@
       <c r="H11" s="137"/>
       <c r="I11" s="137"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>32</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>26/01/2021</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
         <v>28</v>
       </c>
@@ -3562,7 +3565,7 @@
         <v>ASTM D4318, D4943</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
@@ -3572,7 +3575,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="76"/>
       <c r="B15" s="76"/>
       <c r="C15" s="77"/>
@@ -3583,7 +3586,7 @@
       <c r="H15" s="79"/>
       <c r="I15" s="80"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="69" t="s">
         <v>3</v>
       </c>
@@ -3611,7 +3614,7 @@
       <c r="H16" s="69"/>
       <c r="I16" s="83"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="69" t="s">
         <v>5</v>
       </c>
@@ -3639,7 +3642,7 @@
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="69" t="s">
         <v>17</v>
       </c>
@@ -3667,7 +3670,7 @@
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="69" t="s">
         <v>18</v>
       </c>
@@ -3695,7 +3698,7 @@
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
     </row>
-    <row r="20" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="69" t="s">
         <v>51</v>
       </c>
@@ -3723,7 +3726,7 @@
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
     </row>
-    <row r="21" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="69" t="s">
         <v>52</v>
       </c>
@@ -3751,7 +3754,7 @@
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="69" t="s">
         <v>7</v>
       </c>
@@ -3779,7 +3782,7 @@
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="84"/>
       <c r="B23" s="84"/>
       <c r="C23" s="84"/>
@@ -3790,7 +3793,7 @@
       <c r="H23" s="84"/>
       <c r="I23" s="83"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="84"/>
       <c r="B24" s="84"/>
       <c r="C24" s="84"/>
@@ -3801,7 +3804,7 @@
       <c r="H24" s="84"/>
       <c r="I24" s="83"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="83"/>
       <c r="B25" s="83"/>
       <c r="C25" s="83"/>
@@ -3812,7 +3815,7 @@
       <c r="H25" s="83"/>
       <c r="I25" s="83"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="83"/>
       <c r="B26" s="83"/>
       <c r="C26" s="83"/>
@@ -3823,7 +3826,7 @@
       <c r="H26" s="83"/>
       <c r="I26" s="83"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="83"/>
       <c r="B27" s="83"/>
       <c r="C27" s="83"/>
@@ -3834,7 +3837,7 @@
       <c r="H27" s="83"/>
       <c r="I27" s="83"/>
     </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="80"/>
       <c r="B28" s="80"/>
       <c r="C28" s="80"/>
@@ -3845,7 +3848,7 @@
       <c r="H28" s="82"/>
       <c r="I28" s="80"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="80"/>
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
@@ -3856,7 +3859,7 @@
       <c r="H29" s="80"/>
       <c r="I29" s="80"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="80"/>
       <c r="B30" s="80"/>
       <c r="C30" s="80"/>
@@ -3867,10 +3870,10 @@
       <c r="H30" s="80"/>
       <c r="I30" s="80"/>
     </row>
-    <row r="35" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="124" t="s">
         <v>55</v>
       </c>
@@ -3891,34 +3894,34 @@
       </c>
       <c r="I36" s="68"/>
     </row>
-    <row r="37" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
     </row>
-    <row r="38" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="D40" s="17"/>
       <c r="G40" s="19"/>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D41" s="17"/>
       <c r="G41" s="58"/>
     </row>
-    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="17"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -3938,7 +3941,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>5</v>
       </c>
@@ -3958,7 +3961,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>9</v>
       </c>
@@ -3985,7 +3988,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
@@ -4012,7 +4015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>11</v>
       </c>
@@ -4039,7 +4042,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>12</v>
       </c>
@@ -4059,7 +4062,7 @@
       </c>
       <c r="G48" s="16"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>23.844282238442823</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="41"/>
@@ -4086,7 +4089,7 @@
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>58</v>
       </c>
@@ -4098,7 +4101,7 @@
       <c r="G51" s="71"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
       <c r="B52" s="41"/>
       <c r="C52" s="71"/>
@@ -4106,7 +4109,7 @@
       <c r="E52" s="48"/>
       <c r="F52" s="48"/>
     </row>
-    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="106" t="str">
         <f>main!I25</f>
         <v>Shrinkage Limit (%):</v>
@@ -4128,7 +4131,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="106" t="str">
         <f>main!I26</f>
         <v>Shrinkage Ratio:</v>
@@ -4147,7 +4150,7 @@
       <c r="H54" s="140"/>
       <c r="I54" s="141"/>
     </row>
-    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="106" t="str">
         <f>main!I27</f>
         <v>Volumetric Shrinkage (%):</v>
@@ -4169,7 +4172,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="106" t="str">
         <f>main!I28</f>
         <v>Linear Shrinkage (%):</v>
@@ -4191,7 +4194,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="138" t="s">
         <v>70</v>
       </c>
@@ -4207,7 +4210,7 @@
       <c r="H57" s="24"/>
       <c r="I57" s="24"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="24" t="s">
         <v>20</v>
       </c>
@@ -4219,9 +4222,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="str">
         <f>main!A61</f>
         <v>Dr. A. B. M. Badruzzaman</v>
@@ -4232,7 +4235,7 @@
         <v>Dr. Md. Ferdous Alam</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="str">
         <f>main!A62</f>
         <v>Professor</v>
@@ -4243,7 +4246,7 @@
         <v>Assistant Professor</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="str">
         <f>main!A63</f>
         <v>Department of Civil Engineering</v>
@@ -4254,7 +4257,7 @@
         <v>Department of Civil Engineering</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
         <f>main!A64</f>
         <v>BUET, Dhaka - 1000.</v>
@@ -4265,31 +4268,31 @@
         <v>BUET, Dhaka - 1000.</v>
       </c>
     </row>
-    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H127" s="1"/>
     </row>
-    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H129" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H130" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H131" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H133" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
30 data added successfully
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0753d6b33ebe78a/Desktop/thesis-repo/ann-thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0753d6b33ebe78a/Desktop/ann-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A03704-6F40-4749-A219-2C9DF3D8BF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7995" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="50" r:id="rId1"/>
@@ -1402,16 +1402,16 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1423,19 +1423,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.986361813076606</c:v>
+                  <c:v>38.904438224710134</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.427734375000007</c:v>
+                  <c:v>38.278046962355553</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.530214424951282</c:v>
+                  <c:v>38.222903102259693</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.103182256509136</c:v>
+                  <c:v>36.896689270043872</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.6826241134752</c:v>
+                  <c:v>36.11003487020534</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2053,94 +2053,94 @@
             <v>15</v>
           </cell>
           <cell r="E24">
-            <v>19</v>
+            <v>20</v>
           </cell>
           <cell r="F24">
-            <v>24</v>
+            <v>25</v>
           </cell>
           <cell r="G24">
-            <v>29</v>
+            <v>30</v>
           </cell>
           <cell r="H24">
-            <v>34</v>
+            <v>35</v>
           </cell>
           <cell r="M24">
-            <v>7.02</v>
+            <v>9.3699999999999992</v>
           </cell>
           <cell r="N24">
-            <v>11.18</v>
+            <v>10.64</v>
           </cell>
           <cell r="O24">
-            <v>9.09</v>
+            <v>10.4</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25">
-            <v>10.16</v>
+            <v>7.5</v>
           </cell>
           <cell r="E25">
-            <v>8.9600000000000009</v>
+            <v>7.06</v>
           </cell>
           <cell r="F25">
-            <v>9.83</v>
+            <v>6.87</v>
           </cell>
           <cell r="G25">
-            <v>9.6999999999999993</v>
+            <v>6.78</v>
           </cell>
           <cell r="H25">
-            <v>10.23</v>
+            <v>11.21</v>
           </cell>
           <cell r="M25">
-            <v>45.45</v>
+            <v>54.15</v>
           </cell>
           <cell r="N25">
-            <v>47.74</v>
+            <v>52.71</v>
           </cell>
           <cell r="O25">
-            <v>44.72</v>
+            <v>48.7</v>
           </cell>
         </row>
         <row r="26">
           <cell r="D26">
-            <v>44.56</v>
+            <v>42.24</v>
           </cell>
           <cell r="E26">
-            <v>37.31</v>
+            <v>44.16</v>
           </cell>
           <cell r="F26">
-            <v>44.85</v>
+            <v>42.96</v>
           </cell>
           <cell r="G26">
-            <v>38.549999999999997</v>
+            <v>41.1</v>
           </cell>
           <cell r="H26">
-            <v>40.840000000000003</v>
+            <v>46.34</v>
           </cell>
           <cell r="M26">
-            <v>38</v>
+            <v>45.03</v>
           </cell>
           <cell r="N26">
-            <v>40.659999999999997</v>
+            <v>44.1</v>
           </cell>
           <cell r="O26">
-            <v>37.86</v>
+            <v>40.96</v>
           </cell>
         </row>
         <row r="27">
           <cell r="D27">
-            <v>35.090000000000003</v>
+            <v>32.51</v>
           </cell>
           <cell r="E27">
-            <v>29.44</v>
+            <v>33.89</v>
           </cell>
           <cell r="F27">
-            <v>35.479999999999997</v>
+            <v>32.979999999999997</v>
           </cell>
           <cell r="G27">
-            <v>30.44</v>
+            <v>31.85</v>
           </cell>
           <cell r="H27">
-            <v>32.79</v>
+            <v>37.020000000000003</v>
           </cell>
         </row>
       </sheetData>
@@ -2504,7 +2504,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
@@ -2675,19 +2675,19 @@
       </c>
       <c r="D16" s="33">
         <f>'[1]input-output'!$E$24</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="33">
         <f>'[1]input-output'!$F$24</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="33">
         <f>'[1]input-output'!$G$24</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G16" s="33">
         <f>'[1]input-output'!$H$24</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="92" t="s">
@@ -2704,23 +2704,23 @@
       <c r="B17" s="4"/>
       <c r="C17" s="34">
         <f>'[1]input-output'!$D$25</f>
-        <v>10.16</v>
+        <v>7.5</v>
       </c>
       <c r="D17" s="34">
         <f>'[1]input-output'!$E$25</f>
-        <v>8.9600000000000009</v>
+        <v>7.06</v>
       </c>
       <c r="E17" s="34">
         <f>'[1]input-output'!$F$25</f>
-        <v>9.83</v>
+        <v>6.87</v>
       </c>
       <c r="F17" s="34">
         <f>'[1]input-output'!$G$25</f>
-        <v>9.6999999999999993</v>
+        <v>6.78</v>
       </c>
       <c r="G17" s="34">
         <f>'[1]input-output'!$H$25</f>
-        <v>10.23</v>
+        <v>11.21</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2737,23 +2737,23 @@
       <c r="B18" s="12"/>
       <c r="C18" s="34">
         <f>'[1]input-output'!$D$26</f>
-        <v>44.56</v>
+        <v>42.24</v>
       </c>
       <c r="D18" s="34">
         <f>'[1]input-output'!$E$26</f>
-        <v>37.31</v>
+        <v>44.16</v>
       </c>
       <c r="E18" s="34">
         <f>'[1]input-output'!$F$26</f>
-        <v>44.85</v>
+        <v>42.96</v>
       </c>
       <c r="F18" s="34">
         <f>'[1]input-output'!$G$26</f>
-        <v>38.549999999999997</v>
+        <v>41.1</v>
       </c>
       <c r="G18" s="34">
         <f>'[1]input-output'!$H$26</f>
-        <v>40.840000000000003</v>
+        <v>46.34</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2770,23 +2770,23 @@
       <c r="B19" s="4"/>
       <c r="C19" s="34">
         <f>'[1]input-output'!$D$27</f>
-        <v>35.090000000000003</v>
+        <v>32.51</v>
       </c>
       <c r="D19" s="34">
         <f>'[1]input-output'!$E$27</f>
-        <v>29.44</v>
+        <v>33.89</v>
       </c>
       <c r="E19" s="34">
         <f>'[1]input-output'!$F$27</f>
-        <v>35.479999999999997</v>
+        <v>32.979999999999997</v>
       </c>
       <c r="F19" s="34">
         <f>'[1]input-output'!$G$27</f>
-        <v>30.44</v>
+        <v>31.85</v>
       </c>
       <c r="G19" s="34">
         <f>'[1]input-output'!$H$27</f>
-        <v>32.79</v>
+        <v>37.020000000000003</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2803,23 +2803,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>9.4699999999999989</v>
+        <v>9.730000000000004</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>7.870000000000001</v>
+        <v>10.269999999999996</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>9.3700000000000045</v>
+        <v>9.980000000000004</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>8.1099999999999959</v>
+        <v>9.25</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>8.0500000000000043</v>
+        <v>9.32</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2836,23 +2836,23 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>24.930000000000003</v>
+        <v>25.009999999999998</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>20.48</v>
+        <v>26.830000000000002</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>25.65</v>
+        <v>26.109999999999996</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>20.740000000000002</v>
+        <v>25.07</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>22.56</v>
+        <v>25.810000000000002</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2872,23 +2872,23 @@
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>37.986361813076606</v>
+        <v>38.904438224710134</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>38.427734375000007</v>
+        <v>38.278046962355553</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>36.530214424951282</v>
+        <v>38.222903102259693</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>39.103182256509136</v>
+        <v>36.896689270043872</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>35.6826241134752</v>
+        <v>36.11003487020534</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -3059,7 +3059,7 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>3.142590140844304</v>
+        <v>1.6330589712127015</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -3074,7 +3074,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -3092,7 +3092,7 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>4.1367150717615866</v>
+        <v>7.3481730981759092</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -3126,15 +3126,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="36">
         <f>'[1]input-output'!$M$24</f>
-        <v>7.02</v>
+        <v>9.3699999999999992</v>
       </c>
       <c r="E44" s="36">
         <f>'[1]input-output'!$N$24</f>
-        <v>11.18</v>
+        <v>10.64</v>
       </c>
       <c r="F44" s="34">
         <f>'[1]input-output'!$O$24</f>
-        <v>9.09</v>
+        <v>10.4</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3146,15 +3146,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="36">
         <f>'[1]input-output'!$M$25</f>
-        <v>45.45</v>
+        <v>54.15</v>
       </c>
       <c r="E45" s="36">
         <f>'[1]input-output'!$N$25</f>
-        <v>47.74</v>
+        <v>52.71</v>
       </c>
       <c r="F45" s="34">
         <f>'[1]input-output'!$O$25</f>
-        <v>44.72</v>
+        <v>48.7</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3166,15 +3166,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="36">
         <f>'[1]input-output'!$M$26</f>
-        <v>38</v>
+        <v>45.03</v>
       </c>
       <c r="E46" s="36">
         <f>'[1]input-output'!$N$26</f>
-        <v>40.659999999999997</v>
+        <v>44.1</v>
       </c>
       <c r="F46" s="34">
         <f>'[1]input-output'!$O$26</f>
-        <v>37.86</v>
+        <v>40.96</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3186,15 +3186,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>7.4500000000000028</v>
+        <v>9.1199999999999974</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>7.0800000000000054</v>
+        <v>8.61</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>6.8599999999999994</v>
+        <v>7.740000000000002</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3206,15 +3206,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>30.98</v>
+        <v>35.660000000000004</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>29.479999999999997</v>
+        <v>33.46</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>28.77</v>
+        <v>30.560000000000002</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -3226,15 +3226,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>24.047772756617181</v>
+        <v>25.574873808188435</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>24.016282225237472</v>
+        <v>25.732217573221757</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>23.844282238442823</v>
+        <v>25.327225130890056</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -3276,7 +3276,7 @@
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
@@ -3296,7 +3296,7 @@
       <c r="F56" s="63"/>
       <c r="G56" s="67">
         <f>G40-G54</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>13</v>
@@ -3425,7 +3425,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A7:I133"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="C31" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C31" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -3597,19 +3597,19 @@
       </c>
       <c r="D16" s="70">
         <f>main!D16</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="70">
         <f>main!E16</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="70">
         <f>main!F16</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G16" s="70">
         <f>main!G16</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H16" s="69"/>
       <c r="I16" s="83"/>
@@ -3621,23 +3621,23 @@
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>10.16</v>
+        <v>7.5</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>8.9600000000000009</v>
+        <v>7.06</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>9.83</v>
+        <v>6.87</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>9.6999999999999993</v>
+        <v>6.78</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>10.23</v>
+        <v>11.21</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
@@ -3649,23 +3649,23 @@
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>44.56</v>
+        <v>42.24</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>37.31</v>
+        <v>44.16</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>44.85</v>
+        <v>42.96</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>38.549999999999997</v>
+        <v>41.1</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>40.840000000000003</v>
+        <v>46.34</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
@@ -3677,23 +3677,23 @@
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>35.090000000000003</v>
+        <v>32.51</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>29.44</v>
+        <v>33.89</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>35.479999999999997</v>
+        <v>32.979999999999997</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>30.44</v>
+        <v>31.85</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>32.79</v>
+        <v>37.020000000000003</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
@@ -3705,23 +3705,23 @@
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>9.4699999999999989</v>
+        <v>9.730000000000004</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>7.870000000000001</v>
+        <v>10.269999999999996</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>9.3700000000000045</v>
+        <v>9.980000000000004</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>8.1099999999999959</v>
+        <v>9.25</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>8.0500000000000043</v>
+        <v>9.32</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
@@ -3733,23 +3733,23 @@
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>24.930000000000003</v>
+        <v>25.009999999999998</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>20.48</v>
+        <v>26.830000000000002</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>25.65</v>
+        <v>26.109999999999996</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>20.740000000000002</v>
+        <v>25.07</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>22.56</v>
+        <v>25.810000000000002</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
@@ -3761,23 +3761,23 @@
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>37.986361813076606</v>
+        <v>38.904438224710134</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>38.427734375000007</v>
+        <v>38.278046962355553</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>36.530214424951282</v>
+        <v>38.222903102259693</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>39.103182256509136</v>
+        <v>36.896689270043872</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>35.6826241134752</v>
+        <v>36.11003487020534</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
@@ -3881,7 +3881,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3890,7 +3890,7 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>4.1399999999999997</v>
+        <v>7.35</v>
       </c>
       <c r="I36" s="68"/>
     </row>
@@ -3949,15 +3949,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>7.02</v>
+        <v>9.3699999999999992</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>11.18</v>
+        <v>10.64</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>9.09</v>
+        <v>10.4</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3969,15 +3969,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>45.45</v>
+        <v>54.15</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>47.74</v>
+        <v>52.71</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>44.72</v>
+        <v>48.7</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3985,7 +3985,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3996,15 +3996,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>38</v>
+        <v>45.03</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>40.659999999999997</v>
+        <v>44.1</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>37.86</v>
+        <v>40.96</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -4012,7 +4012,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="121">
         <f>main!G56</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -4023,15 +4023,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>7.4500000000000028</v>
+        <v>9.1199999999999974</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>7.0800000000000054</v>
+        <v>8.61</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>6.8599999999999994</v>
+        <v>7.740000000000002</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -4039,7 +4039,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>3.14</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4050,15 +4050,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>30.98</v>
+        <v>35.660000000000004</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>29.479999999999997</v>
+        <v>33.46</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>28.77</v>
+        <v>30.560000000000002</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -4070,15 +4070,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>24.047772756617181</v>
+        <v>25.574873808188435</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>24.016282225237472</v>
+        <v>25.732217573221757</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>23.844282238442823</v>
+        <v>25.327225130890056</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
@@ -4202,7 +4202,7 @@
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.24299999999999999</v>
+        <v>0.252</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>

</xml_diff>

<commit_message>
40 data successfully added from minhaz's pc
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A03704-6F40-4749-A219-2C9DF3D8BF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7995" tabRatio="842" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7995" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="50" r:id="rId1"/>
@@ -1402,13 +1402,13 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>35</c:v>
@@ -1423,19 +1423,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>38.904438224710134</c:v>
+                  <c:v>36.444273042807566</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.278046962355553</c:v>
+                  <c:v>35.065394132202172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.222903102259693</c:v>
+                  <c:v>34.516479536399856</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.896689270043872</c:v>
+                  <c:v>33.845029239766077</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.11003487020534</c:v>
+                  <c:v>33.557760453579021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2053,94 +2053,94 @@
             <v>15</v>
           </cell>
           <cell r="E24">
-            <v>20</v>
+            <v>19</v>
           </cell>
           <cell r="F24">
-            <v>25</v>
+            <v>24</v>
           </cell>
           <cell r="G24">
-            <v>30</v>
+            <v>29</v>
           </cell>
           <cell r="H24">
             <v>35</v>
           </cell>
           <cell r="M24">
-            <v>9.3699999999999992</v>
+            <v>7.03</v>
           </cell>
           <cell r="N24">
-            <v>10.64</v>
+            <v>7.38</v>
           </cell>
           <cell r="O24">
-            <v>10.4</v>
+            <v>7.43</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25">
-            <v>7.5</v>
+            <v>10.37</v>
           </cell>
           <cell r="E25">
-            <v>7.06</v>
+            <v>7.09</v>
           </cell>
           <cell r="F25">
-            <v>6.87</v>
+            <v>7.54</v>
           </cell>
           <cell r="G25">
-            <v>6.78</v>
+            <v>10.88</v>
           </cell>
           <cell r="H25">
-            <v>11.21</v>
+            <v>9.2100000000000009</v>
           </cell>
           <cell r="M25">
-            <v>54.15</v>
+            <v>40.21</v>
           </cell>
           <cell r="N25">
-            <v>52.71</v>
+            <v>38.86</v>
           </cell>
           <cell r="O25">
-            <v>48.7</v>
+            <v>42.06</v>
           </cell>
         </row>
         <row r="26">
           <cell r="D26">
-            <v>42.24</v>
+            <v>45.75</v>
           </cell>
           <cell r="E26">
-            <v>44.16</v>
+            <v>45.3</v>
           </cell>
           <cell r="F26">
-            <v>42.96</v>
+            <v>44.68</v>
           </cell>
           <cell r="G26">
-            <v>41.1</v>
+            <v>47.5</v>
           </cell>
           <cell r="H26">
-            <v>46.34</v>
+            <v>46.9</v>
           </cell>
           <cell r="M26">
-            <v>45.03</v>
+            <v>34.5</v>
           </cell>
           <cell r="N26">
-            <v>44.1</v>
+            <v>33.369999999999997</v>
           </cell>
           <cell r="O26">
-            <v>40.96</v>
+            <v>36.03</v>
           </cell>
         </row>
         <row r="27">
           <cell r="D27">
-            <v>32.51</v>
+            <v>36.299999999999997</v>
           </cell>
           <cell r="E27">
-            <v>33.89</v>
+            <v>35.380000000000003</v>
           </cell>
           <cell r="F27">
-            <v>32.979999999999997</v>
+            <v>35.15</v>
           </cell>
           <cell r="G27">
-            <v>31.85</v>
+            <v>38.24</v>
           </cell>
           <cell r="H27">
-            <v>37.020000000000003</v>
+            <v>37.43</v>
           </cell>
         </row>
       </sheetData>
@@ -2504,7 +2504,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
@@ -2675,15 +2675,15 @@
       </c>
       <c r="D16" s="33">
         <f>'[1]input-output'!$E$24</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="33">
         <f>'[1]input-output'!$F$24</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="33">
         <f>'[1]input-output'!$G$24</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="33">
         <f>'[1]input-output'!$H$24</f>
@@ -2704,23 +2704,23 @@
       <c r="B17" s="4"/>
       <c r="C17" s="34">
         <f>'[1]input-output'!$D$25</f>
-        <v>7.5</v>
+        <v>10.37</v>
       </c>
       <c r="D17" s="34">
         <f>'[1]input-output'!$E$25</f>
-        <v>7.06</v>
+        <v>7.09</v>
       </c>
       <c r="E17" s="34">
         <f>'[1]input-output'!$F$25</f>
-        <v>6.87</v>
+        <v>7.54</v>
       </c>
       <c r="F17" s="34">
         <f>'[1]input-output'!$G$25</f>
-        <v>6.78</v>
+        <v>10.88</v>
       </c>
       <c r="G17" s="34">
         <f>'[1]input-output'!$H$25</f>
-        <v>11.21</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2737,23 +2737,23 @@
       <c r="B18" s="12"/>
       <c r="C18" s="34">
         <f>'[1]input-output'!$D$26</f>
-        <v>42.24</v>
+        <v>45.75</v>
       </c>
       <c r="D18" s="34">
         <f>'[1]input-output'!$E$26</f>
-        <v>44.16</v>
+        <v>45.3</v>
       </c>
       <c r="E18" s="34">
         <f>'[1]input-output'!$F$26</f>
-        <v>42.96</v>
+        <v>44.68</v>
       </c>
       <c r="F18" s="34">
         <f>'[1]input-output'!$G$26</f>
-        <v>41.1</v>
+        <v>47.5</v>
       </c>
       <c r="G18" s="34">
         <f>'[1]input-output'!$H$26</f>
-        <v>46.34</v>
+        <v>46.9</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2770,23 +2770,23 @@
       <c r="B19" s="4"/>
       <c r="C19" s="34">
         <f>'[1]input-output'!$D$27</f>
-        <v>32.51</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="D19" s="34">
         <f>'[1]input-output'!$E$27</f>
-        <v>33.89</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="E19" s="34">
         <f>'[1]input-output'!$F$27</f>
-        <v>32.979999999999997</v>
+        <v>35.15</v>
       </c>
       <c r="F19" s="34">
         <f>'[1]input-output'!$G$27</f>
-        <v>31.85</v>
+        <v>38.24</v>
       </c>
       <c r="G19" s="34">
         <f>'[1]input-output'!$H$27</f>
-        <v>37.020000000000003</v>
+        <v>37.43</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2803,23 +2803,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>9.730000000000004</v>
+        <v>9.4500000000000028</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>10.269999999999996</v>
+        <v>9.9199999999999946</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>9.980000000000004</v>
+        <v>9.5300000000000011</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>9.25</v>
+        <v>9.259999999999998</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>9.32</v>
+        <v>9.4699999999999989</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2836,23 +2836,23 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>25.009999999999998</v>
+        <v>25.93</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>26.830000000000002</v>
+        <v>28.290000000000003</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>26.109999999999996</v>
+        <v>27.61</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>25.07</v>
+        <v>27.36</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>25.810000000000002</v>
+        <v>28.22</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2872,23 +2872,23 @@
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>38.904438224710134</v>
+        <v>36.444273042807566</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>38.278046962355553</v>
+        <v>35.065394132202172</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>38.222903102259693</v>
+        <v>34.516479536399856</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>36.896689270043872</v>
+        <v>33.845029239766077</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>36.11003487020534</v>
+        <v>33.557760453579021</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -3059,7 +3059,7 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>1.6330589712127015</v>
+        <v>1.6934477293234205</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -3074,7 +3074,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -3092,7 +3092,7 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>7.3481730981759092</v>
+        <v>7.6766467455088572</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -3126,15 +3126,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="36">
         <f>'[1]input-output'!$M$24</f>
-        <v>9.3699999999999992</v>
+        <v>7.03</v>
       </c>
       <c r="E44" s="36">
         <f>'[1]input-output'!$N$24</f>
-        <v>10.64</v>
+        <v>7.38</v>
       </c>
       <c r="F44" s="34">
         <f>'[1]input-output'!$O$24</f>
-        <v>10.4</v>
+        <v>7.43</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3146,15 +3146,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="36">
         <f>'[1]input-output'!$M$25</f>
-        <v>54.15</v>
+        <v>40.21</v>
       </c>
       <c r="E45" s="36">
         <f>'[1]input-output'!$N$25</f>
-        <v>52.71</v>
+        <v>38.86</v>
       </c>
       <c r="F45" s="34">
         <f>'[1]input-output'!$O$25</f>
-        <v>48.7</v>
+        <v>42.06</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3166,15 +3166,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="36">
         <f>'[1]input-output'!$M$26</f>
-        <v>45.03</v>
+        <v>34.5</v>
       </c>
       <c r="E46" s="36">
         <f>'[1]input-output'!$N$26</f>
-        <v>44.1</v>
+        <v>33.369999999999997</v>
       </c>
       <c r="F46" s="34">
         <f>'[1]input-output'!$O$26</f>
-        <v>40.96</v>
+        <v>36.03</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3186,15 +3186,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>9.1199999999999974</v>
+        <v>5.7100000000000009</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>8.61</v>
+        <v>5.490000000000002</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>7.740000000000002</v>
+        <v>6.0300000000000011</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3206,15 +3206,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>35.660000000000004</v>
+        <v>27.47</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>33.46</v>
+        <v>25.99</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>30.560000000000002</v>
+        <v>28.6</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -3226,15 +3226,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>25.574873808188435</v>
+        <v>20.786312340735353</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>25.732217573221757</v>
+        <v>21.123509041939219</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>25.327225130890056</v>
+        <v>21.083916083916087</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -3276,7 +3276,7 @@
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
@@ -3296,7 +3296,7 @@
       <c r="F56" s="63"/>
       <c r="G56" s="67">
         <f>G40-G54</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>13</v>
@@ -3425,7 +3425,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A7:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C31" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="C10" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -3597,15 +3597,15 @@
       </c>
       <c r="D16" s="70">
         <f>main!D16</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="70">
         <f>main!E16</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="70">
         <f>main!F16</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="70">
         <f>main!G16</f>
@@ -3621,23 +3621,23 @@
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>7.5</v>
+        <v>10.37</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>7.06</v>
+        <v>7.09</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>6.87</v>
+        <v>7.54</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>6.78</v>
+        <v>10.88</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>11.21</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
@@ -3649,23 +3649,23 @@
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>42.24</v>
+        <v>45.75</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>44.16</v>
+        <v>45.3</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>42.96</v>
+        <v>44.68</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>41.1</v>
+        <v>47.5</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>46.34</v>
+        <v>46.9</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
@@ -3677,23 +3677,23 @@
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>32.51</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>33.89</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>32.979999999999997</v>
+        <v>35.15</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>31.85</v>
+        <v>38.24</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>37.020000000000003</v>
+        <v>37.43</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
@@ -3705,23 +3705,23 @@
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>9.730000000000004</v>
+        <v>9.4500000000000028</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>10.269999999999996</v>
+        <v>9.9199999999999946</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>9.980000000000004</v>
+        <v>9.5300000000000011</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>9.25</v>
+        <v>9.259999999999998</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>9.32</v>
+        <v>9.4699999999999989</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
@@ -3733,23 +3733,23 @@
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>25.009999999999998</v>
+        <v>25.93</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>26.830000000000002</v>
+        <v>28.290000000000003</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>26.109999999999996</v>
+        <v>27.61</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>25.07</v>
+        <v>27.36</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>25.810000000000002</v>
+        <v>28.22</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
@@ -3761,23 +3761,23 @@
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>38.904438224710134</v>
+        <v>36.444273042807566</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>38.278046962355553</v>
+        <v>35.065394132202172</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>38.222903102259693</v>
+        <v>34.516479536399856</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>36.896689270043872</v>
+        <v>33.845029239766077</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>36.11003487020534</v>
+        <v>33.557760453579021</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
@@ -3881,7 +3881,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3890,7 +3890,7 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>7.35</v>
+        <v>7.68</v>
       </c>
       <c r="I36" s="68"/>
     </row>
@@ -3949,15 +3949,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>9.3699999999999992</v>
+        <v>7.03</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>10.64</v>
+        <v>7.38</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>10.4</v>
+        <v>7.43</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3969,15 +3969,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>54.15</v>
+        <v>40.21</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>52.71</v>
+        <v>38.86</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>48.7</v>
+        <v>42.06</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3985,7 +3985,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3996,15 +3996,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>45.03</v>
+        <v>34.5</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>44.1</v>
+        <v>33.369999999999997</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>40.96</v>
+        <v>36.03</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -4012,7 +4012,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="121">
         <f>main!G56</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -4023,15 +4023,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>9.1199999999999974</v>
+        <v>5.7100000000000009</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>8.61</v>
+        <v>5.490000000000002</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>7.740000000000002</v>
+        <v>6.0300000000000011</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -4039,7 +4039,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>1.63</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4050,15 +4050,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>35.660000000000004</v>
+        <v>27.47</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>33.46</v>
+        <v>25.99</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>30.560000000000002</v>
+        <v>28.6</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -4070,15 +4070,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>25.574873808188435</v>
+        <v>20.786312340735353</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>25.732217573221757</v>
+        <v>21.123509041939219</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>25.327225130890056</v>
+        <v>21.083916083916087</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
@@ -4202,7 +4202,7 @@
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.252</v>
+        <v>0.21599999999999997</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>

</xml_diff>

<commit_message>
Mithamain project data collected completely
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D349E95-F1B1-4DF1-BFBF-F633AB6012FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DB9AA4-8520-4E0B-9106-F55FD99A22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1403,7 +1403,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>30</c:v>
@@ -1421,19 +1421,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>40.490797546012281</c:v>
+                  <c:v>46.132037262049373</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.455281560544719</c:v>
+                  <c:v>44.252612448886836</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.058380414312637</c:v>
+                  <c:v>39.42264321154714</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.161010260457751</c:v>
+                  <c:v>42.24173985780007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.510204081632644</c:v>
+                  <c:v>41.332157035730063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,7 +2054,7 @@
             <v>20</v>
           </cell>
           <cell r="F24">
-            <v>24</v>
+            <v>25</v>
           </cell>
           <cell r="G24">
             <v>30</v>
@@ -2063,82 +2063,82 @@
             <v>35</v>
           </cell>
           <cell r="M24">
-            <v>10.07</v>
+            <v>7.1</v>
           </cell>
           <cell r="N24">
-            <v>8.74</v>
+            <v>10.23</v>
           </cell>
           <cell r="O24">
-            <v>9.41</v>
+            <v>9.8000000000000007</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25">
-            <v>10.68</v>
+            <v>7.33</v>
           </cell>
           <cell r="E25">
-            <v>9.98</v>
+            <v>10.83</v>
           </cell>
           <cell r="F25">
-            <v>9.17</v>
+            <v>10.83</v>
           </cell>
           <cell r="G25">
-            <v>9.18</v>
+            <v>7.35</v>
           </cell>
           <cell r="H25">
-            <v>8.99</v>
+            <v>9.0500000000000007</v>
           </cell>
           <cell r="M25">
-            <v>49.01</v>
+            <v>41.97</v>
           </cell>
           <cell r="N25">
-            <v>50.12</v>
+            <v>46.2</v>
           </cell>
           <cell r="O25">
-            <v>47.94</v>
+            <v>43.17</v>
           </cell>
         </row>
         <row r="26">
           <cell r="D26">
-            <v>47.32</v>
+            <v>43.41</v>
           </cell>
           <cell r="E26">
-            <v>47.87</v>
+            <v>42.58</v>
           </cell>
           <cell r="F26">
-            <v>46.09</v>
+            <v>41.74</v>
           </cell>
           <cell r="G26">
-            <v>44.19</v>
+            <v>41.36</v>
           </cell>
           <cell r="H26">
-            <v>42.68</v>
+            <v>41.09</v>
           </cell>
           <cell r="M26">
-            <v>42.12</v>
+            <v>35</v>
           </cell>
           <cell r="N26">
-            <v>42.77</v>
+            <v>38.83</v>
           </cell>
           <cell r="O26">
-            <v>41.09</v>
+            <v>36.39</v>
           </cell>
         </row>
         <row r="27">
           <cell r="D27">
-            <v>36.76</v>
+            <v>32.020000000000003</v>
           </cell>
           <cell r="E27">
-            <v>37.15</v>
+            <v>32.840000000000003</v>
           </cell>
           <cell r="F27">
-            <v>35.72</v>
+            <v>33</v>
           </cell>
           <cell r="G27">
-            <v>34.520000000000003</v>
+            <v>31.26</v>
           </cell>
           <cell r="H27">
-            <v>33.49</v>
+            <v>31.72</v>
           </cell>
         </row>
       </sheetData>
@@ -2502,7 +2502,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="E16" s="33">
         <f>'[1]input-output'!$F$24</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="33">
         <f>'[1]input-output'!$G$24</f>
@@ -2702,23 +2702,23 @@
       <c r="B17" s="4"/>
       <c r="C17" s="34">
         <f>'[1]input-output'!$D$25</f>
-        <v>10.68</v>
+        <v>7.33</v>
       </c>
       <c r="D17" s="34">
         <f>'[1]input-output'!$E$25</f>
-        <v>9.98</v>
+        <v>10.83</v>
       </c>
       <c r="E17" s="34">
         <f>'[1]input-output'!$F$25</f>
-        <v>9.17</v>
+        <v>10.83</v>
       </c>
       <c r="F17" s="34">
         <f>'[1]input-output'!$G$25</f>
-        <v>9.18</v>
+        <v>7.35</v>
       </c>
       <c r="G17" s="34">
         <f>'[1]input-output'!$H$25</f>
-        <v>8.99</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2735,23 +2735,23 @@
       <c r="B18" s="12"/>
       <c r="C18" s="34">
         <f>'[1]input-output'!$D$26</f>
-        <v>47.32</v>
+        <v>43.41</v>
       </c>
       <c r="D18" s="34">
         <f>'[1]input-output'!$E$26</f>
-        <v>47.87</v>
+        <v>42.58</v>
       </c>
       <c r="E18" s="34">
         <f>'[1]input-output'!$F$26</f>
-        <v>46.09</v>
+        <v>41.74</v>
       </c>
       <c r="F18" s="34">
         <f>'[1]input-output'!$G$26</f>
-        <v>44.19</v>
+        <v>41.36</v>
       </c>
       <c r="G18" s="34">
         <f>'[1]input-output'!$H$26</f>
-        <v>42.68</v>
+        <v>41.09</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2768,23 +2768,23 @@
       <c r="B19" s="4"/>
       <c r="C19" s="34">
         <f>'[1]input-output'!$D$27</f>
-        <v>36.76</v>
+        <v>32.020000000000003</v>
       </c>
       <c r="D19" s="34">
         <f>'[1]input-output'!$E$27</f>
-        <v>37.15</v>
+        <v>32.840000000000003</v>
       </c>
       <c r="E19" s="34">
         <f>'[1]input-output'!$F$27</f>
-        <v>35.72</v>
+        <v>33</v>
       </c>
       <c r="F19" s="34">
         <f>'[1]input-output'!$G$27</f>
-        <v>34.520000000000003</v>
+        <v>31.26</v>
       </c>
       <c r="G19" s="34">
         <f>'[1]input-output'!$H$27</f>
-        <v>33.49</v>
+        <v>31.72</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2801,23 +2801,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>10.560000000000002</v>
+        <v>11.389999999999993</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>10.719999999999999</v>
+        <v>9.7399999999999949</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>10.370000000000005</v>
+        <v>8.740000000000002</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>9.6699999999999946</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>9.1899999999999977</v>
+        <v>9.3700000000000045</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2834,23 +2834,23 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>26.08</v>
+        <v>24.690000000000005</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>27.169999999999998</v>
+        <v>22.010000000000005</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>26.549999999999997</v>
+        <v>22.17</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>25.340000000000003</v>
+        <v>23.910000000000004</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>24.5</v>
+        <v>22.669999999999998</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2870,23 +2870,23 @@
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>40.490797546012281</v>
+        <v>46.132037262049373</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>39.455281560544719</v>
+        <v>44.252612448886836</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>39.058380414312637</v>
+        <v>39.42264321154714</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>38.161010260457751</v>
+        <v>42.24173985780007</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>37.510204081632644</v>
+        <v>41.332157035730063</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -3057,7 +3057,7 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>2.1420600057956811</v>
+        <v>1.2486435612943532</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -3072,7 +3072,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -3090,7 +3090,7 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>7.9362856101154122</v>
+        <v>13.614774085230275</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.3">
@@ -3124,15 +3124,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="36">
         <f>'[1]input-output'!$M$24</f>
-        <v>10.07</v>
+        <v>7.1</v>
       </c>
       <c r="E44" s="36">
         <f>'[1]input-output'!$N$24</f>
-        <v>8.74</v>
+        <v>10.23</v>
       </c>
       <c r="F44" s="34">
         <f>'[1]input-output'!$O$24</f>
-        <v>9.41</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3144,15 +3144,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="36">
         <f>'[1]input-output'!$M$25</f>
-        <v>49.01</v>
+        <v>41.97</v>
       </c>
       <c r="E45" s="36">
         <f>'[1]input-output'!$N$25</f>
-        <v>50.12</v>
+        <v>46.2</v>
       </c>
       <c r="F45" s="34">
         <f>'[1]input-output'!$O$25</f>
-        <v>47.94</v>
+        <v>43.17</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3164,15 +3164,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="36">
         <f>'[1]input-output'!$M$26</f>
-        <v>42.12</v>
+        <v>35</v>
       </c>
       <c r="E46" s="36">
         <f>'[1]input-output'!$N$26</f>
-        <v>42.77</v>
+        <v>38.83</v>
       </c>
       <c r="F46" s="34">
         <f>'[1]input-output'!$O$26</f>
-        <v>41.09</v>
+        <v>36.39</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3184,15 +3184,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>6.8900000000000006</v>
+        <v>6.9699999999999989</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>7.3499999999999943</v>
+        <v>7.3700000000000045</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>6.8499999999999943</v>
+        <v>6.7800000000000011</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3204,15 +3204,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>32.049999999999997</v>
+        <v>27.9</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>34.03</v>
+        <v>28.599999999999998</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>31.680000000000003</v>
+        <v>26.59</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -3224,15 +3224,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>21.497659906396262</v>
+        <v>24.982078853046591</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>21.598589479870686</v>
+        <v>25.769230769230788</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>21.622474747474726</v>
+        <v>25.498307634449048</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="E16" s="70">
         <f>main!E16</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="70">
         <f>main!F16</f>
@@ -3619,23 +3619,23 @@
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>10.68</v>
+        <v>7.33</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>9.98</v>
+        <v>10.83</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>9.17</v>
+        <v>10.83</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>9.18</v>
+        <v>7.35</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>8.99</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
@@ -3647,23 +3647,23 @@
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>47.32</v>
+        <v>43.41</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>47.87</v>
+        <v>42.58</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>46.09</v>
+        <v>41.74</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>44.19</v>
+        <v>41.36</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>42.68</v>
+        <v>41.09</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
@@ -3675,23 +3675,23 @@
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>36.76</v>
+        <v>32.020000000000003</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>37.15</v>
+        <v>32.840000000000003</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>35.72</v>
+        <v>33</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>34.520000000000003</v>
+        <v>31.26</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>33.49</v>
+        <v>31.72</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
@@ -3703,23 +3703,23 @@
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>10.560000000000002</v>
+        <v>11.389999999999993</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>10.719999999999999</v>
+        <v>9.7399999999999949</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>10.370000000000005</v>
+        <v>8.740000000000002</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>9.6699999999999946</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>9.1899999999999977</v>
+        <v>9.3700000000000045</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
@@ -3731,23 +3731,23 @@
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>26.08</v>
+        <v>24.690000000000005</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>27.169999999999998</v>
+        <v>22.010000000000005</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>26.549999999999997</v>
+        <v>22.17</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>25.340000000000003</v>
+        <v>23.910000000000004</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>24.5</v>
+        <v>22.669999999999998</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
@@ -3759,23 +3759,23 @@
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>40.490797546012281</v>
+        <v>46.132037262049373</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>39.455281560544719</v>
+        <v>44.252612448886836</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>39.058380414312637</v>
+        <v>39.42264321154714</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>38.161010260457751</v>
+        <v>42.24173985780007</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>37.510204081632644</v>
+        <v>41.332157035730063</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
@@ -3879,7 +3879,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3888,7 +3888,7 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>7.94</v>
+        <v>13.61</v>
       </c>
       <c r="I36" s="68"/>
     </row>
@@ -3947,15 +3947,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>10.07</v>
+        <v>7.1</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>8.74</v>
+        <v>10.23</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>9.41</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3967,15 +3967,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>49.01</v>
+        <v>41.97</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>50.12</v>
+        <v>46.2</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>47.94</v>
+        <v>43.17</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3983,7 +3983,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -3994,15 +3994,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>42.12</v>
+        <v>35</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>42.77</v>
+        <v>38.83</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>41.09</v>
+        <v>36.39</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -4021,15 +4021,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>6.8900000000000006</v>
+        <v>6.9699999999999989</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>7.3499999999999943</v>
+        <v>7.3700000000000045</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>6.8499999999999943</v>
+        <v>6.7800000000000011</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -4037,7 +4037,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>2.14</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4048,15 +4048,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>32.049999999999997</v>
+        <v>27.9</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>34.03</v>
+        <v>28.599999999999998</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>31.680000000000003</v>
+        <v>26.59</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -4068,15 +4068,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>21.497659906396262</v>
+        <v>24.982078853046591</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>21.598589479870686</v>
+        <v>25.769230769230788</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>21.622474747474726</v>
+        <v>25.498307634449048</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.26099999999999995</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>

</xml_diff>

<commit_message>
25 data from coxbazar project is collected
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DB9AA4-8520-4E0B-9106-F55FD99A22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEBA80D-0F83-4BC8-AB5F-EDAD9F546421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1400,10 +1400,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>30</c:v>
@@ -1421,19 +1421,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>46.132037262049373</c:v>
+                  <c:v>32.680621201890617</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.252612448886836</c:v>
+                  <c:v>31.763879128601541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.42264321154714</c:v>
+                  <c:v>30.683403068340318</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.24173985780007</c:v>
+                  <c:v>29.78578714722882</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.332157035730063</c:v>
+                  <c:v>29.323570432357055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,10 +2051,10 @@
             <v>15</v>
           </cell>
           <cell r="E24">
-            <v>20</v>
+            <v>19</v>
           </cell>
           <cell r="F24">
-            <v>25</v>
+            <v>24</v>
           </cell>
           <cell r="G24">
             <v>30</v>
@@ -2063,82 +2063,82 @@
             <v>35</v>
           </cell>
           <cell r="M24">
-            <v>7.1</v>
+            <v>9.42</v>
           </cell>
           <cell r="N24">
-            <v>10.23</v>
+            <v>10.79</v>
           </cell>
           <cell r="O24">
-            <v>9.8000000000000007</v>
+            <v>9.2200000000000006</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25">
-            <v>7.33</v>
+            <v>9.14</v>
           </cell>
           <cell r="E25">
-            <v>10.83</v>
+            <v>9.11</v>
           </cell>
           <cell r="F25">
-            <v>10.83</v>
+            <v>9.86</v>
           </cell>
           <cell r="G25">
-            <v>7.35</v>
+            <v>9.2899999999999991</v>
           </cell>
           <cell r="H25">
-            <v>9.0500000000000007</v>
+            <v>9.0399999999999991</v>
           </cell>
           <cell r="M25">
-            <v>41.97</v>
+            <v>48.39</v>
           </cell>
           <cell r="N25">
-            <v>46.2</v>
+            <v>53.49</v>
           </cell>
           <cell r="O25">
-            <v>43.17</v>
+            <v>49.69</v>
           </cell>
         </row>
         <row r="26">
           <cell r="D26">
-            <v>43.41</v>
+            <v>48.44</v>
           </cell>
           <cell r="E26">
-            <v>42.58</v>
+            <v>46.61</v>
           </cell>
           <cell r="F26">
-            <v>41.74</v>
+            <v>47.34</v>
           </cell>
           <cell r="G26">
-            <v>41.36</v>
+            <v>47.46</v>
           </cell>
           <cell r="H26">
-            <v>41.09</v>
+            <v>46.13</v>
           </cell>
           <cell r="M26">
-            <v>35</v>
+            <v>42.03</v>
           </cell>
           <cell r="N26">
-            <v>38.83</v>
+            <v>46.41</v>
           </cell>
           <cell r="O26">
-            <v>36.39</v>
+            <v>43.08</v>
           </cell>
         </row>
         <row r="27">
           <cell r="D27">
-            <v>32.020000000000003</v>
+            <v>38.76</v>
           </cell>
           <cell r="E27">
-            <v>32.840000000000003</v>
+            <v>37.57</v>
           </cell>
           <cell r="F27">
-            <v>33</v>
+            <v>38.54</v>
           </cell>
           <cell r="G27">
-            <v>31.26</v>
+            <v>38.700000000000003</v>
           </cell>
           <cell r="H27">
-            <v>31.72</v>
+            <v>37.72</v>
           </cell>
         </row>
       </sheetData>
@@ -2502,7 +2502,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A8:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -2673,11 +2673,11 @@
       </c>
       <c r="D16" s="33">
         <f>'[1]input-output'!$E$24</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="33">
         <f>'[1]input-output'!$F$24</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="33">
         <f>'[1]input-output'!$G$24</f>
@@ -2702,23 +2702,23 @@
       <c r="B17" s="4"/>
       <c r="C17" s="34">
         <f>'[1]input-output'!$D$25</f>
-        <v>7.33</v>
+        <v>9.14</v>
       </c>
       <c r="D17" s="34">
         <f>'[1]input-output'!$E$25</f>
-        <v>10.83</v>
+        <v>9.11</v>
       </c>
       <c r="E17" s="34">
         <f>'[1]input-output'!$F$25</f>
-        <v>10.83</v>
+        <v>9.86</v>
       </c>
       <c r="F17" s="34">
         <f>'[1]input-output'!$G$25</f>
-        <v>7.35</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="G17" s="34">
         <f>'[1]input-output'!$H$25</f>
-        <v>9.0500000000000007</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2735,23 +2735,23 @@
       <c r="B18" s="12"/>
       <c r="C18" s="34">
         <f>'[1]input-output'!$D$26</f>
-        <v>43.41</v>
+        <v>48.44</v>
       </c>
       <c r="D18" s="34">
         <f>'[1]input-output'!$E$26</f>
-        <v>42.58</v>
+        <v>46.61</v>
       </c>
       <c r="E18" s="34">
         <f>'[1]input-output'!$F$26</f>
-        <v>41.74</v>
+        <v>47.34</v>
       </c>
       <c r="F18" s="34">
         <f>'[1]input-output'!$G$26</f>
-        <v>41.36</v>
+        <v>47.46</v>
       </c>
       <c r="G18" s="34">
         <f>'[1]input-output'!$H$26</f>
-        <v>41.09</v>
+        <v>46.13</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2768,23 +2768,23 @@
       <c r="B19" s="4"/>
       <c r="C19" s="34">
         <f>'[1]input-output'!$D$27</f>
-        <v>32.020000000000003</v>
+        <v>38.76</v>
       </c>
       <c r="D19" s="34">
         <f>'[1]input-output'!$E$27</f>
-        <v>32.840000000000003</v>
+        <v>37.57</v>
       </c>
       <c r="E19" s="34">
         <f>'[1]input-output'!$F$27</f>
-        <v>33</v>
+        <v>38.54</v>
       </c>
       <c r="F19" s="34">
         <f>'[1]input-output'!$G$27</f>
-        <v>31.26</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="G19" s="34">
         <f>'[1]input-output'!$H$27</f>
-        <v>31.72</v>
+        <v>37.72</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2801,23 +2801,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>11.389999999999993</v>
+        <v>9.68</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>9.7399999999999949</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>8.740000000000002</v>
+        <v>8.8000000000000043</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>10.099999999999998</v>
+        <v>8.759999999999998</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>9.3700000000000045</v>
+        <v>8.4100000000000037</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2834,23 +2834,23 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>24.690000000000005</v>
+        <v>29.619999999999997</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>22.010000000000005</v>
+        <v>28.46</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>22.17</v>
+        <v>28.68</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>23.910000000000004</v>
+        <v>29.410000000000004</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>22.669999999999998</v>
+        <v>28.68</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2870,23 +2870,23 @@
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>46.132037262049373</v>
+        <v>32.680621201890617</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>44.252612448886836</v>
+        <v>31.763879128601541</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>39.42264321154714</v>
+        <v>30.683403068340318</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>42.24173985780007</v>
+        <v>29.78578714722882</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>41.332157035730063</v>
+        <v>29.323570432357055</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -3057,7 +3057,7 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>1.2486435612943532</v>
+        <v>1.1781331452302948</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -3072,7 +3072,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -3090,7 +3090,7 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>13.614774085230275</v>
+        <v>9.3368054744353888</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.3">
@@ -3124,15 +3124,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="36">
         <f>'[1]input-output'!$M$24</f>
-        <v>7.1</v>
+        <v>9.42</v>
       </c>
       <c r="E44" s="36">
         <f>'[1]input-output'!$N$24</f>
-        <v>10.23</v>
+        <v>10.79</v>
       </c>
       <c r="F44" s="34">
         <f>'[1]input-output'!$O$24</f>
-        <v>9.8000000000000007</v>
+        <v>9.2200000000000006</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3144,15 +3144,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="36">
         <f>'[1]input-output'!$M$25</f>
-        <v>41.97</v>
+        <v>48.39</v>
       </c>
       <c r="E45" s="36">
         <f>'[1]input-output'!$N$25</f>
-        <v>46.2</v>
+        <v>53.49</v>
       </c>
       <c r="F45" s="34">
         <f>'[1]input-output'!$O$25</f>
-        <v>43.17</v>
+        <v>49.69</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3164,15 +3164,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="36">
         <f>'[1]input-output'!$M$26</f>
-        <v>35</v>
+        <v>42.03</v>
       </c>
       <c r="E46" s="36">
         <f>'[1]input-output'!$N$26</f>
-        <v>38.83</v>
+        <v>46.41</v>
       </c>
       <c r="F46" s="34">
         <f>'[1]input-output'!$O$26</f>
-        <v>36.39</v>
+        <v>43.08</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3184,15 +3184,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>6.9699999999999989</v>
+        <v>6.3599999999999994</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>7.3700000000000045</v>
+        <v>7.0800000000000054</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>6.7800000000000011</v>
+        <v>6.6099999999999994</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3204,15 +3204,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>27.9</v>
+        <v>32.61</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>28.599999999999998</v>
+        <v>35.619999999999997</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>26.59</v>
+        <v>33.86</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -3224,15 +3224,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>24.982078853046591</v>
+        <v>19.50321987120515</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>25.769230769230788</v>
+        <v>19.876473891072447</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>25.498307634449048</v>
+        <v>19.521559362079149</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
@@ -3294,7 +3294,7 @@
       <c r="F56" s="63"/>
       <c r="G56" s="67">
         <f>G40-G54</f>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>13</v>
@@ -3595,11 +3595,11 @@
       </c>
       <c r="D16" s="70">
         <f>main!D16</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="70">
         <f>main!E16</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="70">
         <f>main!F16</f>
@@ -3619,23 +3619,23 @@
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>7.33</v>
+        <v>9.14</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>10.83</v>
+        <v>9.11</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>10.83</v>
+        <v>9.86</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>7.35</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>9.0500000000000007</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
@@ -3647,23 +3647,23 @@
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>43.41</v>
+        <v>48.44</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>42.58</v>
+        <v>46.61</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>41.74</v>
+        <v>47.34</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>41.36</v>
+        <v>47.46</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>41.09</v>
+        <v>46.13</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
@@ -3675,23 +3675,23 @@
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>32.020000000000003</v>
+        <v>38.76</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>32.840000000000003</v>
+        <v>37.57</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>33</v>
+        <v>38.54</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>31.26</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>31.72</v>
+        <v>37.72</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
@@ -3703,23 +3703,23 @@
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>11.389999999999993</v>
+        <v>9.68</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>9.7399999999999949</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>8.740000000000002</v>
+        <v>8.8000000000000043</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>10.099999999999998</v>
+        <v>8.759999999999998</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>9.3700000000000045</v>
+        <v>8.4100000000000037</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
@@ -3731,23 +3731,23 @@
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>24.690000000000005</v>
+        <v>29.619999999999997</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>22.010000000000005</v>
+        <v>28.46</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>22.17</v>
+        <v>28.68</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>23.910000000000004</v>
+        <v>29.410000000000004</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>22.669999999999998</v>
+        <v>28.68</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
@@ -3759,23 +3759,23 @@
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>46.132037262049373</v>
+        <v>32.680621201890617</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>44.252612448886836</v>
+        <v>31.763879128601541</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>39.42264321154714</v>
+        <v>30.683403068340318</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>42.24173985780007</v>
+        <v>29.78578714722882</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>41.332157035730063</v>
+        <v>29.323570432357055</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
@@ -3879,7 +3879,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3888,7 +3888,7 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>13.61</v>
+        <v>9.34</v>
       </c>
       <c r="I36" s="68"/>
     </row>
@@ -3947,15 +3947,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>7.1</v>
+        <v>9.42</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>10.23</v>
+        <v>10.79</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>9.8000000000000007</v>
+        <v>9.2200000000000006</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3967,15 +3967,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>41.97</v>
+        <v>48.39</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>46.2</v>
+        <v>53.49</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>43.17</v>
+        <v>49.69</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3983,7 +3983,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -3994,15 +3994,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>35</v>
+        <v>42.03</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>38.83</v>
+        <v>46.41</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>36.39</v>
+        <v>43.08</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -4010,7 +4010,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="121">
         <f>main!G56</f>
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -4021,15 +4021,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>6.9699999999999989</v>
+        <v>6.3599999999999994</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>7.3700000000000045</v>
+        <v>7.0800000000000054</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>6.7800000000000011</v>
+        <v>6.6099999999999994</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -4037,7 +4037,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4048,15 +4048,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>27.9</v>
+        <v>32.61</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>28.599999999999998</v>
+        <v>35.619999999999997</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>26.59</v>
+        <v>33.86</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -4068,15 +4068,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>24.982078853046591</v>
+        <v>19.50321987120515</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>25.769230769230788</v>
+        <v>19.876473891072447</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>25.498307634449048</v>
+        <v>19.521559362079149</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.28799999999999998</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>

</xml_diff>

<commit_message>
Total 140 data has been collected successfully
</commit_message>
<xml_diff>
--- a/Limits-V5.xlsx
+++ b/Limits-V5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEBA80D-0F83-4BC8-AB5F-EDAD9F546421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74787106-2A35-4E34-B873-09E510AE8EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1400,10 +1400,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>30</c:v>
@@ -1421,19 +1421,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>32.680621201890617</c:v>
+                  <c:v>32.276250880902055</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.763879128601541</c:v>
+                  <c:v>30.074677528852678</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.683403068340318</c:v>
+                  <c:v>29.464285714285737</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.78578714722882</c:v>
+                  <c:v>28.676716917922956</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.323570432357055</c:v>
+                  <c:v>28.037686809616645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,10 +2051,10 @@
             <v>15</v>
           </cell>
           <cell r="E24">
-            <v>19</v>
+            <v>21</v>
           </cell>
           <cell r="F24">
-            <v>24</v>
+            <v>25</v>
           </cell>
           <cell r="G24">
             <v>30</v>
@@ -2063,82 +2063,82 @@
             <v>35</v>
           </cell>
           <cell r="M24">
-            <v>9.42</v>
+            <v>10.47</v>
           </cell>
           <cell r="N24">
-            <v>10.79</v>
+            <v>9.2899999999999991</v>
           </cell>
           <cell r="O24">
-            <v>9.2200000000000006</v>
+            <v>9.64</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25">
-            <v>9.14</v>
+            <v>10.199999999999999</v>
           </cell>
           <cell r="E25">
-            <v>9.11</v>
+            <v>9.1199999999999992</v>
           </cell>
           <cell r="F25">
-            <v>9.86</v>
+            <v>10</v>
           </cell>
           <cell r="G25">
-            <v>9.2899999999999991</v>
+            <v>9.8699999999999992</v>
           </cell>
           <cell r="H25">
-            <v>9.0399999999999991</v>
+            <v>10.3</v>
           </cell>
           <cell r="M25">
-            <v>48.39</v>
+            <v>52.4</v>
           </cell>
           <cell r="N25">
-            <v>53.49</v>
+            <v>49.54</v>
           </cell>
           <cell r="O25">
-            <v>49.69</v>
+            <v>48.02</v>
           </cell>
         </row>
         <row r="26">
           <cell r="D26">
-            <v>48.44</v>
+            <v>47.74</v>
           </cell>
           <cell r="E26">
-            <v>46.61</v>
+            <v>47.44</v>
           </cell>
           <cell r="F26">
-            <v>47.34</v>
+            <v>47.7</v>
           </cell>
           <cell r="G26">
-            <v>47.46</v>
+            <v>48.28</v>
           </cell>
           <cell r="H26">
-            <v>46.13</v>
+            <v>49.71</v>
           </cell>
           <cell r="M26">
-            <v>42.03</v>
+            <v>46.54</v>
           </cell>
           <cell r="N26">
-            <v>46.41</v>
+            <v>44.02</v>
           </cell>
           <cell r="O26">
-            <v>43.08</v>
+            <v>42.67</v>
           </cell>
         </row>
         <row r="27">
           <cell r="D27">
-            <v>38.76</v>
+            <v>38.58</v>
           </cell>
           <cell r="E27">
-            <v>37.57</v>
+            <v>38.58</v>
           </cell>
           <cell r="F27">
-            <v>38.54</v>
+            <v>39.119999999999997</v>
           </cell>
           <cell r="G27">
-            <v>38.700000000000003</v>
+            <v>39.72</v>
           </cell>
           <cell r="H27">
-            <v>37.72</v>
+            <v>41.08</v>
           </cell>
         </row>
       </sheetData>
@@ -2673,11 +2673,11 @@
       </c>
       <c r="D16" s="33">
         <f>'[1]input-output'!$E$24</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E16" s="33">
         <f>'[1]input-output'!$F$24</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="33">
         <f>'[1]input-output'!$G$24</f>
@@ -2702,23 +2702,23 @@
       <c r="B17" s="4"/>
       <c r="C17" s="34">
         <f>'[1]input-output'!$D$25</f>
-        <v>9.14</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D17" s="34">
         <f>'[1]input-output'!$E$25</f>
-        <v>9.11</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="E17" s="34">
         <f>'[1]input-output'!$F$25</f>
-        <v>9.86</v>
+        <v>10</v>
       </c>
       <c r="F17" s="34">
         <f>'[1]input-output'!$G$25</f>
-        <v>9.2899999999999991</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="G17" s="34">
         <f>'[1]input-output'!$H$25</f>
-        <v>9.0399999999999991</v>
+        <v>10.3</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="92" t="s">
@@ -2735,23 +2735,23 @@
       <c r="B18" s="12"/>
       <c r="C18" s="34">
         <f>'[1]input-output'!$D$26</f>
-        <v>48.44</v>
+        <v>47.74</v>
       </c>
       <c r="D18" s="34">
         <f>'[1]input-output'!$E$26</f>
-        <v>46.61</v>
+        <v>47.44</v>
       </c>
       <c r="E18" s="34">
         <f>'[1]input-output'!$F$26</f>
-        <v>47.34</v>
+        <v>47.7</v>
       </c>
       <c r="F18" s="34">
         <f>'[1]input-output'!$G$26</f>
-        <v>47.46</v>
+        <v>48.28</v>
       </c>
       <c r="G18" s="34">
         <f>'[1]input-output'!$H$26</f>
-        <v>46.13</v>
+        <v>49.71</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="92" t="s">
@@ -2768,23 +2768,23 @@
       <c r="B19" s="4"/>
       <c r="C19" s="34">
         <f>'[1]input-output'!$D$27</f>
-        <v>38.76</v>
+        <v>38.58</v>
       </c>
       <c r="D19" s="34">
         <f>'[1]input-output'!$E$27</f>
-        <v>37.57</v>
+        <v>38.58</v>
       </c>
       <c r="E19" s="34">
         <f>'[1]input-output'!$F$27</f>
-        <v>38.54</v>
+        <v>39.119999999999997</v>
       </c>
       <c r="F19" s="34">
         <f>'[1]input-output'!$G$27</f>
-        <v>38.700000000000003</v>
+        <v>39.72</v>
       </c>
       <c r="G19" s="34">
         <f>'[1]input-output'!$H$27</f>
-        <v>37.72</v>
+        <v>41.08</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="92" t="s">
@@ -2801,23 +2801,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4">
         <f>C18-C19</f>
-        <v>9.68</v>
+        <v>9.1600000000000037</v>
       </c>
       <c r="D20" s="4">
         <f>D18-D19</f>
-        <v>9.0399999999999991</v>
+        <v>8.86</v>
       </c>
       <c r="E20" s="4">
         <f>E18-E19</f>
-        <v>8.8000000000000043</v>
+        <v>8.5800000000000054</v>
       </c>
       <c r="F20" s="4">
         <f>F18-F19</f>
-        <v>8.759999999999998</v>
+        <v>8.5600000000000023</v>
       </c>
       <c r="G20" s="4">
         <f>G18-G19</f>
-        <v>8.4100000000000037</v>
+        <v>8.6300000000000026</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="92" t="s">
@@ -2834,23 +2834,23 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <f>C19-C17</f>
-        <v>29.619999999999997</v>
+        <v>28.38</v>
       </c>
       <c r="D21" s="4">
         <f>D19-D17</f>
-        <v>28.46</v>
+        <v>29.46</v>
       </c>
       <c r="E21" s="4">
         <f>E19-E17</f>
-        <v>28.68</v>
+        <v>29.119999999999997</v>
       </c>
       <c r="F21" s="4">
         <f>F19-F17</f>
-        <v>29.410000000000004</v>
+        <v>29.85</v>
       </c>
       <c r="G21" s="4">
         <f>G19-G17</f>
-        <v>28.68</v>
+        <v>30.779999999999998</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="92" t="s">
@@ -2870,23 +2870,23 @@
       <c r="B22" s="4"/>
       <c r="C22" s="31">
         <f>C20/C21*100</f>
-        <v>32.680621201890617</v>
+        <v>32.276250880902055</v>
       </c>
       <c r="D22" s="31">
         <f>D20/D21*100</f>
-        <v>31.763879128601541</v>
+        <v>30.074677528852678</v>
       </c>
       <c r="E22" s="31">
         <f>E20/E21*100</f>
-        <v>30.683403068340318</v>
+        <v>29.464285714285737</v>
       </c>
       <c r="F22" s="31">
         <f>F20/F21*100</f>
-        <v>29.78578714722882</v>
+        <v>28.676716917922956</v>
       </c>
       <c r="G22" s="31">
         <f>G20/G21*100</f>
-        <v>29.323570432357055</v>
+        <v>28.037686809616645</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="92" t="s">
@@ -3057,7 +3057,7 @@
       <c r="F39" s="63"/>
       <c r="G39" s="64">
         <f>G56/G41</f>
-        <v>1.1781331452302948</v>
+        <v>1.2360727390012112</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -3072,7 +3072,7 @@
       <c r="F40" s="63"/>
       <c r="G40" s="65">
         <f>ROUND(TREND(C22:G22,LOG10(C16:G16),LOG10(25)),0)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
@@ -3090,7 +3090,7 @@
       <c r="F41" s="63"/>
       <c r="G41" s="64">
         <f>(TREND(C22:G22,LOG10(C16:G16),LOG10(20))-TREND(C22:G22,LOG10(C16:G16),LOG10(30)))/(LOG10(30)-LOG10(20))</f>
-        <v>9.3368054744353888</v>
+        <v>11.326194291213376</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.3">
@@ -3124,15 +3124,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="36">
         <f>'[1]input-output'!$M$24</f>
-        <v>9.42</v>
+        <v>10.47</v>
       </c>
       <c r="E44" s="36">
         <f>'[1]input-output'!$N$24</f>
-        <v>10.79</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="F44" s="34">
         <f>'[1]input-output'!$O$24</f>
-        <v>9.2200000000000006</v>
+        <v>9.64</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3144,15 +3144,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="36">
         <f>'[1]input-output'!$M$25</f>
-        <v>48.39</v>
+        <v>52.4</v>
       </c>
       <c r="E45" s="36">
         <f>'[1]input-output'!$N$25</f>
-        <v>53.49</v>
+        <v>49.54</v>
       </c>
       <c r="F45" s="34">
         <f>'[1]input-output'!$O$25</f>
-        <v>49.69</v>
+        <v>48.02</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -3164,15 +3164,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="36">
         <f>'[1]input-output'!$M$26</f>
-        <v>42.03</v>
+        <v>46.54</v>
       </c>
       <c r="E46" s="36">
         <f>'[1]input-output'!$N$26</f>
-        <v>46.41</v>
+        <v>44.02</v>
       </c>
       <c r="F46" s="34">
         <f>'[1]input-output'!$O$26</f>
-        <v>43.08</v>
+        <v>42.67</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3184,15 +3184,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="4">
         <f>D45-D46</f>
-        <v>6.3599999999999994</v>
+        <v>5.8599999999999994</v>
       </c>
       <c r="E47" s="4">
         <f>E45-E46</f>
-        <v>7.0800000000000054</v>
+        <v>5.519999999999996</v>
       </c>
       <c r="F47" s="4">
         <f>F45-F46</f>
-        <v>6.6099999999999994</v>
+        <v>5.3500000000000014</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3204,15 +3204,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="4">
         <f>D46-D44</f>
-        <v>32.61</v>
+        <v>36.07</v>
       </c>
       <c r="E48" s="4">
         <f>E46-E44</f>
-        <v>35.619999999999997</v>
+        <v>34.730000000000004</v>
       </c>
       <c r="F48" s="4">
         <f>F46-F44</f>
-        <v>33.86</v>
+        <v>33.03</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -3224,15 +3224,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="31">
         <f>D47/D48*100</f>
-        <v>19.50321987120515</v>
+        <v>16.24618796784031</v>
       </c>
       <c r="E49" s="31">
         <f>E47/E48*100</f>
-        <v>19.876473891072447</v>
+        <v>15.894039735099325</v>
       </c>
       <c r="F49" s="31">
         <f>F47/F48*100</f>
-        <v>19.521559362079149</v>
+        <v>16.197396306388136</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
       <c r="F54" s="63"/>
       <c r="G54" s="67">
         <f>ROUND((D49+E49+F49)/3,0)</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>13</v>
@@ -3294,7 +3294,7 @@
       <c r="F56" s="63"/>
       <c r="G56" s="67">
         <f>G40-G54</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>13</v>
@@ -3595,11 +3595,11 @@
       </c>
       <c r="D16" s="70">
         <f>main!D16</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E16" s="70">
         <f>main!E16</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="70">
         <f>main!F16</f>
@@ -3619,23 +3619,23 @@
       <c r="B17" s="69"/>
       <c r="C17" s="70">
         <f>main!C17</f>
-        <v>9.14</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D17" s="70">
         <f>main!D17</f>
-        <v>9.11</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="E17" s="70">
         <f>main!E17</f>
-        <v>9.86</v>
+        <v>10</v>
       </c>
       <c r="F17" s="70">
         <f>main!F17</f>
-        <v>9.2899999999999991</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="G17" s="70">
         <f>main!G17</f>
-        <v>9.0399999999999991</v>
+        <v>10.3</v>
       </c>
       <c r="H17" s="69"/>
       <c r="I17" s="83"/>
@@ -3647,23 +3647,23 @@
       <c r="B18" s="69"/>
       <c r="C18" s="70">
         <f>main!C18</f>
-        <v>48.44</v>
+        <v>47.74</v>
       </c>
       <c r="D18" s="70">
         <f>main!D18</f>
-        <v>46.61</v>
+        <v>47.44</v>
       </c>
       <c r="E18" s="70">
         <f>main!E18</f>
-        <v>47.34</v>
+        <v>47.7</v>
       </c>
       <c r="F18" s="70">
         <f>main!F18</f>
-        <v>47.46</v>
+        <v>48.28</v>
       </c>
       <c r="G18" s="70">
         <f>main!G18</f>
-        <v>46.13</v>
+        <v>49.71</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="83"/>
@@ -3675,23 +3675,23 @@
       <c r="B19" s="69"/>
       <c r="C19" s="70">
         <f>main!C19</f>
-        <v>38.76</v>
+        <v>38.58</v>
       </c>
       <c r="D19" s="70">
         <f>main!D19</f>
-        <v>37.57</v>
+        <v>38.58</v>
       </c>
       <c r="E19" s="70">
         <f>main!E19</f>
-        <v>38.54</v>
+        <v>39.119999999999997</v>
       </c>
       <c r="F19" s="70">
         <f>main!F19</f>
-        <v>38.700000000000003</v>
+        <v>39.72</v>
       </c>
       <c r="G19" s="70">
         <f>main!G19</f>
-        <v>37.72</v>
+        <v>41.08</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="83"/>
@@ -3703,23 +3703,23 @@
       <c r="B20" s="69"/>
       <c r="C20" s="70">
         <f>main!C20</f>
-        <v>9.68</v>
+        <v>9.1600000000000037</v>
       </c>
       <c r="D20" s="70">
         <f>main!D20</f>
-        <v>9.0399999999999991</v>
+        <v>8.86</v>
       </c>
       <c r="E20" s="70">
         <f>main!E20</f>
-        <v>8.8000000000000043</v>
+        <v>8.5800000000000054</v>
       </c>
       <c r="F20" s="70">
         <f>main!F20</f>
-        <v>8.759999999999998</v>
+        <v>8.5600000000000023</v>
       </c>
       <c r="G20" s="70">
         <f>main!G20</f>
-        <v>8.4100000000000037</v>
+        <v>8.6300000000000026</v>
       </c>
       <c r="H20" s="69"/>
       <c r="I20" s="83"/>
@@ -3731,23 +3731,23 @@
       <c r="B21" s="69"/>
       <c r="C21" s="70">
         <f>main!C21</f>
-        <v>29.619999999999997</v>
+        <v>28.38</v>
       </c>
       <c r="D21" s="70">
         <f>main!D21</f>
-        <v>28.46</v>
+        <v>29.46</v>
       </c>
       <c r="E21" s="70">
         <f>main!E21</f>
-        <v>28.68</v>
+        <v>29.119999999999997</v>
       </c>
       <c r="F21" s="70">
         <f>main!F21</f>
-        <v>29.410000000000004</v>
+        <v>29.85</v>
       </c>
       <c r="G21" s="70">
         <f>main!G21</f>
-        <v>28.68</v>
+        <v>30.779999999999998</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="83"/>
@@ -3759,23 +3759,23 @@
       <c r="B22" s="69"/>
       <c r="C22" s="70">
         <f>main!C22</f>
-        <v>32.680621201890617</v>
+        <v>32.276250880902055</v>
       </c>
       <c r="D22" s="70">
         <f>main!D22</f>
-        <v>31.763879128601541</v>
+        <v>30.074677528852678</v>
       </c>
       <c r="E22" s="70">
         <f>main!E22</f>
-        <v>30.683403068340318</v>
+        <v>29.464285714285737</v>
       </c>
       <c r="F22" s="70">
         <f>main!F22</f>
-        <v>29.78578714722882</v>
+        <v>28.676716917922956</v>
       </c>
       <c r="G22" s="70">
         <f>main!G22</f>
-        <v>29.323570432357055</v>
+        <v>28.037686809616645</v>
       </c>
       <c r="H22" s="69"/>
       <c r="I22" s="83"/>
@@ -3879,7 +3879,7 @@
       <c r="C36" s="68"/>
       <c r="D36" s="122">
         <f>main!G40</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="124" t="s">
@@ -3888,7 +3888,7 @@
       <c r="G36" s="68"/>
       <c r="H36" s="123">
         <f>ROUND(main!G41,2)</f>
-        <v>9.34</v>
+        <v>11.33</v>
       </c>
       <c r="I36" s="68"/>
     </row>
@@ -3947,15 +3947,15 @@
       <c r="C44" s="9"/>
       <c r="D44" s="86">
         <f>main!D44</f>
-        <v>9.42</v>
+        <v>10.47</v>
       </c>
       <c r="E44" s="86">
         <f>main!E44</f>
-        <v>10.79</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="F44" s="86">
         <f>main!F44</f>
-        <v>9.2200000000000006</v>
+        <v>9.64</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3967,15 +3967,15 @@
       <c r="C45" s="7"/>
       <c r="D45" s="86">
         <f>main!D45</f>
-        <v>48.39</v>
+        <v>52.4</v>
       </c>
       <c r="E45" s="86">
         <f>main!E45</f>
-        <v>53.49</v>
+        <v>49.54</v>
       </c>
       <c r="F45" s="86">
         <f>main!F45</f>
-        <v>49.69</v>
+        <v>48.02</v>
       </c>
       <c r="G45" s="106" t="s">
         <v>56</v>
@@ -3983,7 +3983,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="121">
         <f>main!G54</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -3994,15 +3994,15 @@
       <c r="C46" s="27"/>
       <c r="D46" s="86">
         <f>main!D46</f>
-        <v>42.03</v>
+        <v>46.54</v>
       </c>
       <c r="E46" s="86">
         <f>main!E46</f>
-        <v>46.41</v>
+        <v>44.02</v>
       </c>
       <c r="F46" s="86">
         <f>main!F46</f>
-        <v>43.08</v>
+        <v>42.67</v>
       </c>
       <c r="G46" s="106" t="s">
         <v>57</v>
@@ -4010,7 +4010,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="121">
         <f>main!G56</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -4021,15 +4021,15 @@
       <c r="C47" s="26"/>
       <c r="D47" s="86">
         <f>main!D47</f>
-        <v>6.3599999999999994</v>
+        <v>5.8599999999999994</v>
       </c>
       <c r="E47" s="86">
         <f>main!E47</f>
-        <v>7.0800000000000054</v>
+        <v>5.519999999999996</v>
       </c>
       <c r="F47" s="86">
         <f>main!F47</f>
-        <v>6.6099999999999994</v>
+        <v>5.3500000000000014</v>
       </c>
       <c r="G47" s="106" t="s">
         <v>54</v>
@@ -4037,7 +4037,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="109">
         <f>ROUND(main!G39,2)</f>
-        <v>1.18</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4048,15 +4048,15 @@
       <c r="C48" s="7"/>
       <c r="D48" s="86">
         <f>main!D48</f>
-        <v>32.61</v>
+        <v>36.07</v>
       </c>
       <c r="E48" s="86">
         <f>main!E48</f>
-        <v>35.619999999999997</v>
+        <v>34.730000000000004</v>
       </c>
       <c r="F48" s="86">
         <f>main!F48</f>
-        <v>33.86</v>
+        <v>33.03</v>
       </c>
       <c r="G48" s="16"/>
     </row>
@@ -4068,15 +4068,15 @@
       <c r="C49" s="7"/>
       <c r="D49" s="86">
         <f>main!D49</f>
-        <v>19.50321987120515</v>
+        <v>16.24618796784031</v>
       </c>
       <c r="E49" s="86">
         <f>main!E49</f>
-        <v>19.876473891072447</v>
+        <v>15.894039735099325</v>
       </c>
       <c r="F49" s="86">
         <f>main!F49</f>
-        <v>19.521559362079149</v>
+        <v>16.197396306388136</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
       <c r="C57" s="117"/>
       <c r="D57" s="118">
         <f>0.009*(D36-10)</f>
-        <v>0.18899999999999997</v>
+        <v>0.18</v>
       </c>
       <c r="E57" s="119"/>
       <c r="F57" s="120"/>

</xml_diff>